<commit_message>
adicionando os testes de newsletter
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -502,22 +502,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 1d</t>
+          <t>🟢 1d 12h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🟢 9h 37m</t>
+          <t>🟢 16h 22m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 4h 24m</t>
+          <t>🟢 5h 9m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🔵 10h 50m</t>
+          <t>🟡 14h 32m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -566,27 +566,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🔵 5d 18h</t>
+          <t>🟡 8d 1h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 7h 25m</t>
+          <t>🟢 10h 10m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🔴 1d 2h</t>
+          <t>🔴 1d 15h</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🔴 1d 10h</t>
+          <t>🔴 2d 2h</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>🟡 2d 22h</t>
+          <t>🟡 3d 21h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -630,22 +630,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟢 17h 32m</t>
+          <t>🟢 1d</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 6h 53m</t>
+          <t>🟢 10h 5m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 4h 31m</t>
+          <t>🟢 6h 32m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🔵 6h 8m</t>
+          <t>🔵 7h 31m</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -694,42 +694,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>🟡 8d 15h</t>
+          <t>🔴 12d 21h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>🟢 2h 24m</t>
+          <t>🟢 3h 51m</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🔵 10h 49m</t>
+          <t>🟡 18h 6m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🔵 6h 29m</t>
+          <t>🔵 7h 56m</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>🔴 7d 19h</t>
+          <t>🔴 11d 15h</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🟡 17.56%</t>
+          <t>🟡 17.64%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🔵 2.3%</t>
+          <t>🔵 2.22%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>80.15% - 17.56% - 2.3%</t>
+          <t>80.15% - 17.64% - 2.22%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -738,10 +738,10 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -758,27 +758,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🔵 4d 17h</t>
+          <t>🟡 6d 20h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🟢 13h 58m</t>
+          <t>🟢 17h 24m</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 3h 40m</t>
+          <t>🟢 4h 22m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 9h 8m</t>
+          <t>🟡 14h 38m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>🟡 3d 14h</t>
+          <t>🟡 5d 8h</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -802,16 +802,16 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -822,42 +822,42 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 8d 2h</t>
+          <t>🟡 12d 4h</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🔵 21h 18m</t>
+          <t>🔵 1d 5h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🟢 4h 48m</t>
+          <t>🟢 5h 27m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🟡 23h 43m</t>
+          <t>🔴 1d 8h</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>🔴 6d</t>
+          <t>🔴 9d 10h</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 21.56%</t>
+          <t>🔴 23.75%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🔵 2.5%</t>
+          <t>🔵 2.72%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>75.94% - 21.56% - 2.5%</t>
+          <t>73.53% - 23.75% - 2.72%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L7" t="n">
         <v>33</v>
@@ -886,27 +886,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 9d 18h</t>
+          <t>🔴 14d 2h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 15h 35m</t>
+          <t>🔵 21h 47m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🔵 11h 47m</t>
+          <t>🟡 18h 6m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🔴 2d</t>
+          <t>🔴 2d 23h</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🔴 6d 14h</t>
+          <t>🔴 9d 10h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -950,12 +950,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🔵 6d 8h</t>
+          <t>🟡 9d 14h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🔵 1d 10h</t>
+          <t>🟡 2d 3h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -965,12 +965,12 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🔵 6h 43m</t>
+          <t>🔵 7h 59m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>🟡 4d 14h</t>
+          <t>🔴 7d 2h</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1014,27 +1014,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 7d 10h</t>
+          <t>🟡 10d 20h</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 9h 56m</t>
+          <t>🟢 14h 36m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 3h 48m</t>
+          <t>🟢 5h 8m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 4h 47m</t>
+          <t>🔵 6h 46m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 6d 15h</t>
+          <t>🔴 9d 17h</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -1058,10 +1058,10 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -1078,42 +1078,42 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🔵 6d 4h</t>
+          <t>🟡 9d 2h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 14h 35m</t>
+          <t>🔵 20h 19m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🔵 7h 2m</t>
+          <t>🔵 10h 1m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 1d 2h</t>
+          <t>🔴 1d 13h</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🟡 4d 5h</t>
+          <t>🔴 6d 7h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🔵 11.38%</t>
+          <t>🔵 12.11%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🔴 8.13%</t>
+          <t>🔴 8.2%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>80.49% - 11.38% - 8.13%</t>
+          <t>79.69% - 12.11% - 8.2%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
@@ -1142,42 +1142,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 6d 22h</t>
+          <t>🟡 10d 4h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🟢 8h 46m</t>
+          <t>🟢 11h 57m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 6h 5m</t>
+          <t>🔵 9h 12m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 6h 48m</t>
+          <t>🔵 9h 46m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 6d</t>
+          <t>🔴 8d 21h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🔵 9.16%</t>
+          <t>🔵 9.19%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 13.39%</t>
+          <t>🔴 13.36%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>77.45% - 9.16% - 13.39%</t>
+          <t>77.45% - 9.19% - 13.36%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1186,13 +1186,13 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -1206,27 +1206,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 3d 16h</t>
+          <t>🔵 5d 13h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🔵 22h 15m</t>
+          <t>🔵 1d 9h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 2h 46m</t>
+          <t>🟢 3h 9m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🔵 8h 46m</t>
+          <t>🔵 11h 15m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>🟡 2d 7h</t>
+          <t>🟡 3d 13h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1270,27 +1270,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>🔵 5d 18h</t>
+          <t>🟡 8d 1h</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🟢 7h 25m</t>
+          <t>🟢 10h 10m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🔴 1d 2h</t>
+          <t>🔴 1d 15h</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>🔴 1d 10h</t>
+          <t>🔴 2d 2h</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>🟡 2d 22h</t>
+          <t>🟡 3d 21h</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1470,22 +1470,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 1d 14h</t>
+          <t>🟢 1d 22h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🟢 18h 12m</t>
+          <t>🔵 23h 59m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 2h 38m</t>
+          <t>🟢 3h 20m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🟡 17h 48m</t>
+          <t>🟡 19h 18m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1495,22 +1495,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 4.58%</t>
+          <t>🟢 4.53%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 12.06%</t>
+          <t>🔴 12.33%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>83.36% - 4.58% - 12.06%</t>
+          <t>83.14% - 4.53% - 12.33%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>11 (8 - 3 - 0)</t>
+          <t>14 (10 - 4 - 0)</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1527,22 +1527,22 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>⬇ + 13h 47m</t>
+          <t>⬇ + 10h 34m</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>⬇ + 8h 35m</t>
+          <t>⬇ + 7h 37m</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>⬆ - 1h 46m</t>
+          <t>⬆ - 1h 49m</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>⬇ + 6h 58m</t>
+          <t>⬇ + 4h 46m</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -1552,12 +1552,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>⬇ + 0.27%</t>
+          <t>⬇ + 0.22%</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>⬆ - 29.64%</t>
+          <t>⬆ - 29.37%</t>
         </is>
       </c>
       <c r="V2" t="n">
@@ -1575,47 +1575,47 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🟡 7d 16h</t>
+          <t>🟡 9d 20h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🔵 23h 43m</t>
+          <t>🟢 17h 14m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🟢 4h</t>
+          <t>🟢 5h 14m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🟡 16h 26m</t>
+          <t>🟡 15h 59m</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>🔴 5d 20h</t>
+          <t>🔴 8d 6h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🔵 11.93%</t>
+          <t>🔵 9.35%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>🔴 14.94%</t>
+          <t>🔴 22.59%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>73.13% - 11.93% - 14.94%</t>
+          <t>68.06% - 9.35% - 22.59%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>28 (13 - 9 - 6)</t>
+          <t>36 (17 - 11 - 8)</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -1632,37 +1632,37 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>⬇ + 1d 22h</t>
+          <t>⬇ + 1d 19h</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>⬇ + 16h 18m</t>
+          <t>⬇ + 7h 4m</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>⬆ - 22h 21m</t>
+          <t>⬆ - 1d 10h</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>⬆ - 17h 34m</t>
+          <t>⬆ - 1d 10h</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>⬇ + 2d 21h</t>
+          <t>⬇ + 4d 9h</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>⬆ - 11.1%</t>
+          <t>⬆ - 13.68%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>⬇ + 10.81%</t>
+          <t>⬇ + 18.46%</t>
         </is>
       </c>
       <c r="V3" t="n">
@@ -1680,47 +1680,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🔵 5d 2h</t>
+          <t>🟡 7d 21h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 6h 59m</t>
+          <t>🟢 9h 1m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 4h 2m</t>
+          <t>🟢 4h 26m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🟢 2h 18m</t>
+          <t>🟢 4h 5m</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>🟡 4d 12h</t>
+          <t>🔴 7d 3h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🔵 9.1%</t>
+          <t>🔵 14.14%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🔴 7.25%</t>
+          <t>🟡 6.89%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>83.65% - 9.1% - 7.25%</t>
+          <t>78.97% - 14.14% - 6.89%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>48 (25 - 19 - 4)</t>
+          <t>57 (29 - 24 - 4)</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1737,37 +1737,37 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>⬇ + 4d 8h</t>
+          <t>⬇ + 6d 20h</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>⬇ + 6m</t>
+          <t>⬆ - 1h 4m</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>⬆ - 29m</t>
+          <t>⬆ - 2h 6m</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>⬆ - 3h 50m</t>
+          <t>⬆ - 3h 26m</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>⬇ + 4d 12h</t>
+          <t>⬇ + 7d 3h</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>⬇ + 4.44%</t>
+          <t>⬇ + 9.48%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>⬆ - 8.95%</t>
+          <t>⬆ - 9.31%</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -1787,54 +1787,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>🟢 16h 41m</t>
+          <t>🔴 14d 8h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>🟢 5m</t>
+          <t>🔵 1d 16h</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🟢 55m</t>
+          <t>🟢 1h 5m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🟡 15h 41m</t>
+          <t>🟡 21h 26m</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>⚪ 0m</t>
+          <t>🔴 11d 18h</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🔵 14.9%</t>
+          <t>🟡 15.23%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🔵 4.91%</t>
+          <t>🔵 4.79%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>80.19% - 14.9% - 4.91%</t>
+          <t>79.99% - 15.23% - 4.79%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>16 (8 - 6 - 2)</t>
+          <t>22 (14 - 6 - 2)</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L5" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1844,41 +1844,43 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>⬆ - 7d 22h</t>
+          <t>⬇ + 1d 11h</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>⬆ - 2h 19m</t>
+          <t>⬇ + 1d 12h</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>⬆ - 9h 54m</t>
+          <t>⬆ - 17h 1m</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>⬇ + 9h 12m</t>
+          <t>⬇ + 13h 30m</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>⬆ - 7d 19h</t>
+          <t>⬇ + 2h 55m</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>⬆ - 2.66%</t>
+          <t>⬆ - 2.41%</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>⬇ + 2.61%</t>
-        </is>
-      </c>
-      <c r="V5" t="n">
-        <v/>
+          <t>⬇ + 2.57%</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>⬆ - 11.0</t>
+        </is>
       </c>
       <c r="W5" t="n">
         <v/>
@@ -1892,101 +1894,103 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🔵 4d 13h</t>
+          <t>🟡 6d 17h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🟢 17h 57m</t>
+          <t>🔵 1d 11h</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 1h 28m</t>
+          <t>🟢 2h 42m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 12h 45m</t>
+          <t>🟡 16h 20m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>🟡 3d 5h</t>
+          <t>🟡 4d 11h</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 8.54%</t>
+          <t>🟢 7.97%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🔴 7.75%</t>
+          <t>🟡 6.96%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>83.7% - 8.54% - 7.75%</t>
+          <t>85.06% - 7.97% - 6.96%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>69 (38 - 20 - 11)</t>
+          <t>90 (56 - 23 - 11)</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬆ - 3h 50m</t>
+          <t>⬆ - 2h 35m</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>⬇ + 3h 59m</t>
+          <t>⬇ + 18h 16m</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>⬆ - 2h 12m</t>
+          <t>⬆ - 1h 40m</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 3h 37m</t>
+          <t>⬇ + 1h 42m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>⬆ - 9h 14m</t>
+          <t>⬆ - 20h 53m</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>⬇ + 1.55%</t>
+          <t>⬇ + 0.98%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>⬆ - 7.83%</t>
+          <t>⬆ - 8.62%</t>
         </is>
       </c>
       <c r="V6" t="n">
         <v/>
       </c>
-      <c r="W6" t="n">
-        <v/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1997,104 +2001,104 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 11d 10h</t>
+          <t>🔴 16d</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🟢 9h 24m</t>
+          <t>🔵 1d 9h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🔵 8h 36m</t>
+          <t>🔵 11h 56m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🟡 1d</t>
+          <t>🔴 2d</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>🔴 9d 15h</t>
+          <t>🔴 12d 2h</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 35.96%</t>
+          <t>🔴 26.03%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🟡 6.6%</t>
+          <t>🟡 6.33%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>57.44% - 35.96% - 6.6%</t>
+          <t>67.63% - 26.03% - 6.33%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>57 (43 - 12 - 2)</t>
+          <t>68 (49 - 15 - 4)</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="L7" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="M7" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="N7" t="n">
         <v>1</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 3d 7h</t>
+          <t>⬇ + 3d 20h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>⬆ - 11h 54m</t>
+          <t>⬇ + 4h 49m</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>⬇ + 3h 48m</t>
+          <t>⬇ + 6h 29m</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>⬇ + 50m</t>
+          <t>⬇ + 16h 7m</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>⬇ + 3d 15h</t>
+          <t>⬇ + 2d 16h</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>⬇ + 14.4%</t>
+          <t>⬇ + 2.28%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>⬇ + 4.1%</t>
+          <t>⬇ + 3.61%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>⬇ + 5.0</t>
+          <t>⬇ + 3.0</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>⬇ + 9.0</t>
+          <t>⬇ + 11.0</t>
         </is>
       </c>
     </row>
@@ -2106,47 +2110,47 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🔵 6d 7h</t>
+          <t>🟡 8d 21h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 12h 4m</t>
+          <t>🟢 15h 21m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🟢 6h 28m</t>
+          <t>🔵 11h 29m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🔴 1d 5h</t>
+          <t>🔴 1d 12h</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🟡 4d 7h</t>
+          <t>🔴 6d 6h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🔵 13.47%</t>
+          <t>🔵 11.89%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🟡 5.46%</t>
+          <t>🔵 4.5%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>81.07% - 13.47% - 5.46%</t>
+          <t>83.61% - 11.89% - 4.5%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>115 (85 - 18 - 12)</t>
+          <t>152 (112 - 22 - 18)</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -2156,44 +2160,44 @@
         <v>8</v>
       </c>
       <c r="M8" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N8" t="n">
         <v>8</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>⬆ - 3d 11h</t>
+          <t>⬆ - 5d 5h</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 3h 31m</t>
+          <t>⬆ - 6h 26m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 19m</t>
+          <t>⬆ - 6h 37m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>⬆ - 18h 58m</t>
+          <t>⬆ - 1d 11h</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>⬆ - 2d 7h</t>
+          <t>⬆ - 3d 4h</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>⬇ + 5.54%</t>
+          <t>⬇ + 3.96%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>⬆ - 0.21%</t>
+          <t>⬆ - 1.17%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -2203,7 +2207,7 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>⬇ + 4.0</t>
+          <t>⬇ + 5.0</t>
         </is>
       </c>
     </row>
@@ -2215,47 +2219,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🔵 6d</t>
+          <t>🟡 7d 8h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🟡 2d 10h</t>
+          <t>🟡 2d 18h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🟢 3h 4m</t>
+          <t>🟢 2h 14m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🟡 14h 27m</t>
+          <t>🟡 16h 36m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>🟡 2d 20h</t>
+          <t>🟡 3d 18h</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 12.52%</t>
+          <t>🔵 10.62%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🔴 7.76%</t>
+          <t>🔴 7.72%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>79.72% - 12.52% - 7.76%</t>
+          <t>81.66% - 10.62% - 7.72%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>28 (19 - 7 - 2)</t>
+          <t>38 (28 - 8 - 2)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -2272,37 +2276,37 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>⬆ - 7h 51m</t>
+          <t>⬆ - 2d 6h</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>⬇ + 23h 33m</t>
+          <t>⬇ + 15h 14m</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>⬇ + 1h 55m</t>
+          <t>⬇ + 1h 5m</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>⬇ + 7h 44m</t>
+          <t>⬇ + 8h 37m</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>⬆ - 1d 17h</t>
+          <t>⬆ - 3d 7h</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>⬇ + 2.95%</t>
+          <t>⬇ + 1.05%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>⬇ + 4.69%</t>
+          <t>⬇ + 4.65%</t>
         </is>
       </c>
       <c r="V9" t="n">
@@ -2320,54 +2324,54 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟢 7h 22m</t>
+          <t>🟡 8d 19h</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 3h 40m</t>
+          <t>🟢 6h 5m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 41m</t>
+          <t>🟢 1h 7m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 3h 1m</t>
+          <t>🟢 4h 34m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>⚪ 0m</t>
+          <t>🔴 8d 7h</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 2.35%</t>
+          <t>🟢 2.17%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 16.63%</t>
+          <t>🔴 17.03%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>81.02% - 2.35% - 16.63%</t>
+          <t>80.8% - 2.17% - 17.03%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>12 (5 - 7 - 0)</t>
+          <t>18 (6 - 11 - 1)</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="M10" t="n">
         <v>0</v>
@@ -2377,41 +2381,43 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>⬆ - 7d 2h</t>
+          <t>⬆ - 2d</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>⬆ - 6h 16m</t>
+          <t>⬆ - 8h 31m</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>⬆ - 3h 7m</t>
+          <t>⬆ - 4h 1m</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>⬆ - 1h 46m</t>
+          <t>⬆ - 2h 12m</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>⬆ - 6d 15h</t>
+          <t>⬆ - 1d 10h</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>⬆ - 0.59%</t>
+          <t>⬆ - 0.77%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>⬆ - 5.66%</t>
-        </is>
-      </c>
-      <c r="V10" t="n">
-        <v/>
+          <t>⬆ - 5.26%</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>⬇ + 8.0</t>
+        </is>
       </c>
       <c r="W10" t="n">
         <v/>
@@ -2425,104 +2431,102 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 7d 14h</t>
+          <t>🟡 10d 22h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 9h 29m</t>
+          <t>🔵 19h 26m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🟢 6h 22m</t>
+          <t>🔵 9h 17m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 18h 48m</t>
+          <t>🔴 1d 5h</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🔴 6d 3h</t>
+          <t>🔴 8d 12h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🟡 19.51%</t>
+          <t>🟡 17.35%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🟡 6.44%</t>
+          <t>🟡 5.91%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>74.05% - 19.51% - 6.44%</t>
+          <t>76.74% - 17.35% - 5.91%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>220 (153 - 49 - 18)</t>
+          <t>277 (190 - 61 - 26)</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L11" t="n">
         <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="N11" t="n">
         <v>0</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>⬇ + 1d 9h</t>
+          <t>⬇ + 1d 19h</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬆ - 5h 6m</t>
+          <t>⬆ - 53m</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 40m</t>
+          <t>⬆ - 44m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 7h 20m</t>
+          <t>⬆ - 7h 43m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>⬇ + 1d 22h</t>
+          <t>⬇ + 2d 5h</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>⬇ + 8.13%</t>
+          <t>⬇ + 5.24%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>⬆ - 1.69%</t>
-        </is>
-      </c>
-      <c r="V11" t="inlineStr">
-        <is>
-          <t>⬇ + 2.0</t>
-        </is>
+          <t>⬆ - 2.29%</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v/>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>⬇ + 13.0</t>
+          <t>⬇ + 16.0</t>
         </is>
       </c>
     </row>
@@ -2534,101 +2538,105 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟢 1d 20h</t>
+          <t>🟡 9d 23h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🟢 7h 14m</t>
+          <t>🔵 1d 3h</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 1h 1m</t>
+          <t>🟢 1h 38m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 10h 29m</t>
+          <t>🟡 14h 6m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔵 1d 1h</t>
+          <t>🔴 8d 4h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🟢 8.6%</t>
+          <t>🟢 8.46%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 9.76%</t>
+          <t>🔴 9.59%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>81.64% - 8.6% - 9.76%</t>
+          <t>81.95% - 8.46% - 9.59%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>97 (51 - 33 - 13)</t>
+          <t>130 (76 - 40 - 14)</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>⬆ - 5d 1h</t>
+          <t>⬆ - 5h 18m</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>⬆ - 1h 32m</t>
+          <t>⬇ + 15h 18m</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>⬆ - 5h 4m</t>
+          <t>⬆ - 7h 34m</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 3h 41m</t>
+          <t>⬇ + 4h 20m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>⬆ - 4d 22h</t>
+          <t>⬆ - 17h 22m</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>⬆ - 0.56%</t>
+          <t>⬆ - 0.73%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>⬆ - 3.63%</t>
-        </is>
-      </c>
-      <c r="V12" t="n">
-        <v/>
-      </c>
-      <c r="W12" t="n">
-        <v/>
+          <t>⬆ - 3.77%</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>⬆ - 3.0</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2639,47 +2647,47 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 3d 19h</t>
+          <t>🔵 4d 15h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🔵 1d 14h</t>
+          <t>🟡 1d 21h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 2h 51m</t>
+          <t>🟢 2h 47m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🟡 16h 7m</t>
+          <t>🟡 17h 57m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>🔵 1d 10h</t>
+          <t>🔵 1d 21h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 8.55%</t>
+          <t>🟢 7.57%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 9.91%</t>
+          <t>🔴 10.03%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>81.54% - 8.55% - 9.91%</t>
+          <t>82.4% - 7.57% - 10.03%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>39 (27 - 10 - 2)</t>
+          <t>52 (38 - 12 - 2)</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -2696,37 +2704,37 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>⬇ + 2h 58m</t>
+          <t>⬆ - 21h 52m</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>⬇ + 16h 4m</t>
+          <t>⬇ + 11h 25m</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>⬇ + 5m</t>
+          <t>⬆ - 22m</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>⬇ + 7h 21m</t>
+          <t>⬇ + 6h 42m</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>⬆ - 20h 31m</t>
+          <t>⬆ - 1d 15h</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>⬇ + 1.61%</t>
+          <t>⬇ + 0.63%</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>⬆ - 12.47%</t>
+          <t>⬆ - 12.35%</t>
         </is>
       </c>
       <c r="V13" t="n">
@@ -2744,47 +2752,47 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>🟡 7d 16h</t>
+          <t>🟡 9d 20h</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🔵 23h 43m</t>
+          <t>🟢 17h 14m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🟢 4h</t>
+          <t>🟢 5h 14m</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>🟡 16h 26m</t>
+          <t>🟡 15h 59m</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>🔴 5d 20h</t>
+          <t>🔴 8d 6h</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>🔵 11.93%</t>
+          <t>🔵 9.35%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>🔴 14.94%</t>
+          <t>🔴 22.59%</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>73.13% - 11.93% - 14.94%</t>
+          <t>68.06% - 9.35% - 22.59%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>28 (13 - 9 - 6)</t>
+          <t>36 (17 - 11 - 8)</t>
         </is>
       </c>
       <c r="K14" t="n">
@@ -2801,37 +2809,37 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>⬇ + 1d 22h</t>
+          <t>⬇ + 1d 19h</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>⬇ + 16h 18m</t>
+          <t>⬇ + 7h 4m</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>⬆ - 22h 21m</t>
+          <t>⬆ - 1d 10h</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>⬆ - 17h 34m</t>
+          <t>⬆ - 1d 10h</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>⬇ + 2d 21h</t>
+          <t>⬇ + 4d 9h</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>⬆ - 11.1%</t>
+          <t>⬆ - 13.68%</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>⬇ + 10.81%</t>
+          <t>⬇ + 18.46%</t>
         </is>
       </c>
       <c r="V14" t="n">

</xml_diff>

<commit_message>
ajustes na funcao q pega metricas add dados ao template de deck
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -616,10 +616,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -808,10 +808,10 @@
         <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -847,17 +847,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 23.75%</t>
+          <t>🔴 23.4%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🔵 2.72%</t>
+          <t>🔵 2.68%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>73.53% - 23.75% - 2.72%</t>
+          <t>73.92% - 23.4% - 2.68%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1064,10 +1064,10 @@
         <v>13</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
@@ -1103,17 +1103,17 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🔵 12.11%</t>
+          <t>🔵 12.0%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🔴 8.2%</t>
+          <t>🔴 8.18%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>79.69% - 12.11% - 8.2%</t>
+          <t>79.82% - 12.0% - 8.18%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1192,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
@@ -1320,7 +1320,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -1470,22 +1470,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 2d 6h</t>
+          <t>🟢 2d 5h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🔵 1d 9h</t>
+          <t>🔵 1d 8h</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 3h 50m</t>
+          <t>🟢 3h 42m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🟡 17h 11m</t>
+          <t>🟡 17h 12m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1495,22 +1495,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 3.14%</t>
+          <t>🟢 3.71%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 15.62%</t>
+          <t>🔴 15.39%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>81.24% - 3.14% - 15.62%</t>
+          <t>80.9% - 3.71% - 15.39%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>15 (11 - 4 - 0)</t>
+          <t>16 (12 - 4 - 0)</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1527,22 +1527,22 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>⬇ + 18h 40m</t>
+          <t>⬇ + 17h 28m</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>⬇ + 17h 20m</t>
+          <t>⬇ + 16h 15m</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>⬆ - 1h 19m</t>
+          <t>⬆ - 1h 27m</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>⬇ + 2h 39m</t>
+          <t>⬇ + 2h 40m</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -1552,12 +1552,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>⬆ - 1.17%</t>
+          <t>⬆ - 0.6%</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>⬆ - 26.08%</t>
+          <t>⬆ - 26.31%</t>
         </is>
       </c>
       <c r="V2" t="n">
@@ -1615,7 +1615,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>36 (17 - 11 - 8)</t>
+          <t>38 (17 - 12 - 9)</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -1625,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1668,8 +1668,10 @@
       <c r="V3" t="n">
         <v/>
       </c>
-      <c r="W3" t="n">
-        <v/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1680,47 +1682,47 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟡 7d 20h</t>
+          <t>🟡 9d 18h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 8h 21m</t>
+          <t>🟢 8h 9m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 4h 40m</t>
+          <t>🟢 4h 33m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🟢 3h 56m</t>
+          <t>🟢 3h 51m</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>🔴 7d 3h</t>
+          <t>🔴 9d 2h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🟡 19.98%</t>
+          <t>🟡 18.82%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🟡 6.31%</t>
+          <t>🔴 7.02%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>73.72% - 19.98% - 6.31%</t>
+          <t>74.16% - 18.82% - 7.02%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>57 (29 - 24 - 4)</t>
+          <t>64 (30 - 27 - 7)</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -1737,37 +1739,37 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>⬇ + 6d 20h</t>
+          <t>⬇ + 8d 18h</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>⬆ - 1h 44m</t>
+          <t>⬆ - 1h 56m</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>⬆ - 1h 52m</t>
+          <t>⬆ - 1h 59m</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>⬆ - 3h 35m</t>
+          <t>⬆ - 3h 40m</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>⬇ + 7d 3h</t>
+          <t>⬇ + 9d 2h</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>⬇ + 15.32%</t>
+          <t>⬇ + 14.16%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>⬆ - 9.89%</t>
+          <t>⬆ - 9.18%</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -1827,11 +1829,11 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>25 (17 - 6 - 2)</t>
+          <t>27 (17 - 8 - 2)</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L5" t="n">
         <v>16</v>
@@ -1879,7 +1881,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>⬆ - 10.0</t>
+          <t>⬆ - 6.0</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -1894,22 +1896,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🟡 6d 15h</t>
+          <t>🟡 6d 12h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🔵 1d 9h</t>
+          <t>🔵 1d 7h</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 2h 57m</t>
+          <t>🟢 2h 47m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🟡 15h 55m</t>
+          <t>🟡 15h 4m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1919,22 +1921,22 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 7.92%</t>
+          <t>🟢 7.28%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🟡 6.81%</t>
+          <t>🟡 6.26%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>85.27% - 7.92% - 6.81%</t>
+          <t>86.46% - 7.28% - 6.26%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>91 (57 - 23 - 11)</t>
+          <t>92 (58 - 23 - 11)</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -1944,29 +1946,29 @@
         <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬆ - 5h 4m</t>
+          <t>⬆ - 8h 7m</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>⬇ + 15h 57m</t>
+          <t>⬇ + 13h 55m</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>⬆ - 1h 25m</t>
+          <t>⬆ - 1h 35m</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 17m</t>
+          <t>⬇ + 26m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1976,19 +1978,21 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>⬇ + 0.93%</t>
+          <t>⬇ + 0.29%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>⬆ - 8.77%</t>
+          <t>⬆ - 9.32%</t>
         </is>
       </c>
       <c r="V6" t="n">
         <v/>
       </c>
-      <c r="W6" t="n">
-        <v/>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>⬇ + 2.0</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -1999,17 +2003,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🔴 16d 12h</t>
+          <t>🔴 17d 8h</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🔵 1d 12h</t>
+          <t>🟡 2d 5h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🔵 12h 53m</t>
+          <t>🟡 14h 53m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -2024,29 +2028,29 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 24.66%</t>
+          <t>🟡 20.68%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🟡 5.65%</t>
+          <t>🟡 5.56%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>69.69% - 24.66% - 5.65%</t>
+          <t>73.77% - 20.68% - 5.56%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>69 (50 - 15 - 4)</t>
+          <t>70 (51 - 15 - 4)</t>
         </is>
       </c>
       <c r="K7" t="n">
         <v>35</v>
       </c>
       <c r="L7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M7" t="n">
         <v>20</v>
@@ -2056,17 +2060,17 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 4d 8h</t>
+          <t>⬇ + 5d 3h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>⬇ + 6h 56m</t>
+          <t>⬇ + 23h 59m</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>⬇ + 7h 26m</t>
+          <t>⬇ + 9h 26m</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -2081,12 +2085,12 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>⬇ + 0.91%</t>
+          <t>⬆ - 2.72%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>⬇ + 2.93%</t>
+          <t>⬇ + 2.88%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
@@ -2108,22 +2112,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 8d 20h</t>
+          <t>🟡 8d 16h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 14h 34m</t>
+          <t>🟢 13h 22m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🔵 10h 50m</t>
+          <t>🔵 9h 59m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🔴 1d 12h</t>
+          <t>🔴 1d 10h</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2133,22 +2137,22 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🔵 11.86%</t>
+          <t>🔵 11.82%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🔵 4.57%</t>
+          <t>🔵 4.6%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>83.56% - 11.86% - 4.57%</t>
+          <t>83.58% - 11.82% - 4.6%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>156 (115 - 23 - 18)</t>
+          <t>169 (123 - 28 - 18)</t>
         </is>
       </c>
       <c r="K8" t="n">
@@ -2165,22 +2169,22 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>⬆ - 5d 6h</t>
+          <t>⬆ - 5d 10h</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 7h 13m</t>
+          <t>⬆ - 8h 25m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 7h 16m</t>
+          <t>⬆ - 8h 7m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>⬆ - 1d 11h</t>
+          <t>⬆ - 1d 13h</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -2190,12 +2194,12 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>⬇ + 3.93%</t>
+          <t>⬇ + 3.89%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>⬆ - 1.1%</t>
+          <t>⬆ - 1.07%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -2217,22 +2221,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🟡 7d 9h</t>
+          <t>🟡 7d 17h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🟡 2d 18h</t>
+          <t>🟡 2d 22h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🟢 3h 21m</t>
+          <t>🔵 10h 8m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🟡 16h 36m</t>
+          <t>🟡 14h 24m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2242,22 +2246,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 10.62%</t>
+          <t>🔵 9.61%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🔴 7.72%</t>
+          <t>🔴 7.07%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>81.66% - 10.62% - 7.72%</t>
+          <t>83.31% - 9.61% - 7.07%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>38 (28 - 8 - 2)</t>
+          <t>42 (30 - 10 - 2)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -2274,22 +2278,22 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>⬆ - 2d 5h</t>
+          <t>⬆ - 1d 21h</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>⬇ + 15h 14m</t>
+          <t>⬇ + 18h 47m</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>⬇ + 2h 12m</t>
+          <t>⬇ + 8h 59m</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>⬇ + 8h 37m</t>
+          <t>⬇ + 6h 25m</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -2299,12 +2303,12 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>⬇ + 1.05%</t>
+          <t>⬇ + 0.04%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>⬇ + 4.65%</t>
+          <t>⬇ + 4.0%</t>
         </is>
       </c>
       <c r="V9" t="n">
@@ -2322,103 +2326,105 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 10d 1h</t>
+          <t>🟡 8d</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 5h 43m</t>
+          <t>🟢 5h 25m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 1h 3m</t>
+          <t>🟢 58m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 4h 23m</t>
+          <t>🟢 4h 31m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 9d 14h</t>
+          <t>🔴 7d 13h</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 2.68%</t>
+          <t>🟢 5.36%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 17.68%</t>
+          <t>🔴 18.74%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>79.64% - 2.68% - 17.68%</t>
+          <t>75.9% - 5.36% - 18.74%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>19 (6 - 11 - 2)</t>
+          <t>21 (6 - 12 - 3)</t>
         </is>
       </c>
       <c r="K10" t="n">
+        <v>9</v>
+      </c>
+      <c r="L10" t="n">
         <v>12</v>
       </c>
-      <c r="L10" t="n">
-        <v>9</v>
-      </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>⬆ - 18h 35m</t>
+          <t>⬆ - 2d 19h</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>⬆ - 8h 53m</t>
+          <t>⬆ - 9h 11m</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>⬆ - 4h 5m</t>
+          <t>⬆ - 4h 10m</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>⬆ - 2h 23m</t>
+          <t>⬆ - 2h 15m</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>⬆ - 3h 14m</t>
+          <t>⬆ - 2d 4h</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>⬆ - 0.26%</t>
+          <t>⬇ + 2.42%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>⬆ - 4.61%</t>
+          <t>⬆ - 3.55%</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>⬇ + 10.0</t>
-        </is>
-      </c>
-      <c r="W10" t="n">
-        <v/>
+          <t>⬇ + 7.0</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>⬇ + 4.0</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -2429,17 +2435,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 11d 1h</t>
+          <t>🟡 11d 22h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🔵 19h 39m</t>
+          <t>🔵 1d</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🔵 9h 27m</t>
+          <t>🔵 9h 48m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2449,27 +2455,27 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🔴 8d 12h</t>
+          <t>🔴 9d 3h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🟡 18.83%</t>
+          <t>🟡 17.11%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🟡 5.51%</t>
+          <t>🟡 5.72%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>75.66% - 18.83% - 5.51%</t>
+          <t>77.17% - 17.11% - 5.72%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>282 (194 - 62 - 26)</t>
+          <t>303 (204 - 70 - 29)</t>
         </is>
       </c>
       <c r="K11" t="n">
@@ -2486,37 +2492,37 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>⬇ + 1d 23h</t>
+          <t>⬇ + 2d 19h</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬆ - 40m</t>
+          <t>⬇ + 4h 33m</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 34m</t>
+          <t>⬆ - 13m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 4h 37m</t>
+          <t>⬆ - 5h 11m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 5h</t>
+          <t>⬇ + 2d 20h</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>⬇ + 6.72%</t>
+          <t>⬇ + 5.11%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>⬆ - 2.69%</t>
+          <t>⬆ - 2.46%</t>
         </is>
       </c>
       <c r="V11" t="n">
@@ -2536,101 +2542,105 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 10d 2h</t>
+          <t>🟡 9d 9h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🔵 22h 32m</t>
+          <t>🔵 21h 46m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 1h 36m</t>
+          <t>🟢 1h 31m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 11h 52m</t>
+          <t>🔵 11h 38m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 8d 14h</t>
+          <t>🔴 7d 22h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🟢 8.73%</t>
+          <t>🔵 9.41%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 9.68%</t>
+          <t>🔴 9.85%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>81.59% - 8.73% - 9.68%</t>
+          <t>80.74% - 9.41% - 9.85%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>135 (80 - 40 - 15)</t>
+          <t>140 (81 - 43 - 16)</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="N12" t="n">
         <v>0</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>⬆ - 1h 58m</t>
+          <t>⬆ - 19h 25m</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>⬇ + 10h 35m</t>
+          <t>⬇ + 9h 49m</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>⬆ - 7h 36m</t>
+          <t>⬆ - 7h 41m</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 2h 6m</t>
+          <t>⬇ + 1h 52m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>⬆ - 7h 4m</t>
+          <t>⬆ - 23h 25m</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>⬆ - 0.46%</t>
+          <t>⬇ + 0.22%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>⬆ - 3.68%</t>
-        </is>
-      </c>
-      <c r="V12" t="n">
-        <v/>
-      </c>
-      <c r="W12" t="n">
-        <v/>
+          <t>⬆ - 3.51%</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>⬇ + 1.0</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>⬇ + 6.0</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -2641,22 +2651,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 4d 20h</t>
+          <t>🔵 4d 23h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🟡 2d 2h</t>
+          <t>🟡 2d 3h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 3h 35m</t>
+          <t>🟢 6h 55m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🟡 16h 53m</t>
+          <t>🟡 15h 48m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2666,22 +2676,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 6.88%</t>
+          <t>🟢 6.66%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 11.67%</t>
+          <t>🔴 11.24%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>81.45% - 6.88% - 11.67%</t>
+          <t>82.1% - 6.66% - 11.24%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>53 (39 - 12 - 2)</t>
+          <t>58 (42 - 14 - 2)</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -2698,22 +2708,22 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>⬆ - 17h 15m</t>
+          <t>⬆ - 13h 47m</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>⬇ + 16h 17m</t>
+          <t>⬇ + 17h 31m</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>⬇ + 26m</t>
+          <t>⬇ + 3h 46m</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>⬇ + 5h 38m</t>
+          <t>⬇ + 4h 33m</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -2723,12 +2733,12 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>⬆ - 0.06%</t>
+          <t>⬆ - 0.28%</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>⬆ - 10.71%</t>
+          <t>⬆ - 11.14%</t>
         </is>
       </c>
       <c r="V13" t="n">
@@ -2786,7 +2796,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>36 (17 - 11 - 8)</t>
+          <t>38 (17 - 12 - 9)</t>
         </is>
       </c>
       <c r="K14" t="n">
@@ -2796,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="n">
         <v>0</v>
@@ -2839,8 +2849,10 @@
       <c r="V14" t="n">
         <v/>
       </c>
-      <c r="W14" t="n">
-        <v/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix - metricas de bugs e dt de cada tribo agora estão sendo somadas corretamente
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -674,16 +674,16 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -741,7 +741,7 @@
         <v>13</v>
       </c>
       <c r="L5" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -808,7 +808,7 @@
         <v>2</v>
       </c>
       <c r="M6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N6" t="n">
         <v>9</v>
@@ -866,7 +866,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" t="n">
         <v>33</v>
@@ -1058,16 +1058,16 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1122,16 +1122,16 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="M11" t="n">
         <v>9</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1186,16 +1186,16 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="M12" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -1323,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1470,22 +1470,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 2d 5h</t>
+          <t>🟢 2d 4h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🔵 1d 8h</t>
+          <t>🔵 1d 7h</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 3h 42m</t>
+          <t>🟢 3h 34m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🟡 17h 12m</t>
+          <t>🟡 17h 10m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1495,22 +1495,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 3.71%</t>
+          <t>🟢 3.67%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 15.39%</t>
+          <t>🔴 15.46%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>80.9% - 3.71% - 15.39%</t>
+          <t>80.87% - 3.67% - 15.46%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>16 (12 - 4 - 0)</t>
+          <t>17 (12 - 5 - 0)</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1527,22 +1527,22 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>⬇ + 17h 28m</t>
+          <t>⬇ + 16h 8m</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>⬇ + 16h 15m</t>
+          <t>⬇ + 15h 5m</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>⬆ - 1h 27m</t>
+          <t>⬆ - 1h 35m</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>⬇ + 2h 40m</t>
+          <t>⬇ + 2h 38m</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -1552,12 +1552,12 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>⬆ - 0.6%</t>
+          <t>⬆ - 0.64%</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>⬆ - 26.31%</t>
+          <t>⬆ - 26.24%</t>
         </is>
       </c>
       <c r="V2" t="n">
@@ -1575,103 +1575,103 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🟡 9d 20h</t>
+          <t>🟡 9d 6h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 17h 14m</t>
+          <t>🟢 15h 44m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🟢 5h 14m</t>
+          <t>🟢 5h 43m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🟡 15h 59m</t>
+          <t>🔵 13h 49m</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>🔴 8d 6h</t>
+          <t>🔴 7d 19h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🔵 9.35%</t>
+          <t>🔵 9.82%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>🔴 22.59%</t>
+          <t>🔴 22.08%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>68.06% - 9.35% - 22.59%</t>
+          <t>68.1% - 9.82% - 22.08%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>38 (17 - 12 - 9)</t>
+          <t>39 (18 - 12 - 9)</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>⬇ + 1d 19h</t>
+          <t>⬇ + 1d 5h</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>⬇ + 7h 4m</t>
+          <t>⬇ + 5h 34m</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>⬆ - 1d 10h</t>
+          <t>⬆ - 1d 9h</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>⬆ - 1d 10h</t>
+          <t>⬆ - 1d 12h</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>⬇ + 4d 9h</t>
+          <t>⬇ + 3d 21h</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>⬆ - 13.68%</t>
+          <t>⬆ - 13.21%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>⬇ + 18.46%</t>
-        </is>
-      </c>
-      <c r="V3" t="n">
+          <t>⬇ + 17.95%</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>⬇ + 1.0</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
         <v/>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>⬆ - 1.0</t>
-        </is>
       </c>
     </row>
     <row r="4">
@@ -1682,12 +1682,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟡 9d 18h</t>
+          <t>🟡 9d 14h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 8h 9m</t>
+          <t>🟢 10h 6m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1702,22 +1702,22 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>🔴 9d 2h</t>
+          <t>🔴 8d 19h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🟡 18.82%</t>
+          <t>🟡 16.63%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🔴 7.02%</t>
+          <t>🟡 6.2%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>74.16% - 18.82% - 7.02%</t>
+          <t>77.17% - 16.63% - 6.2%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1726,10 +1726,10 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -1739,12 +1739,12 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>⬇ + 8d 18h</t>
+          <t>⬇ + 8d 14h</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>⬆ - 1h 56m</t>
+          <t>⬇ + 1m</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
@@ -1759,23 +1759,21 @@
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>⬇ + 9d 2h</t>
+          <t>⬇ + 8d 19h</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>⬇ + 14.16%</t>
+          <t>⬇ + 11.97%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>⬆ - 9.18%</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>⬆ - 1.0</t>
-        </is>
+          <t>⬆ - 10.0%</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
+        <v/>
       </c>
       <c r="W4" t="n">
         <v/>
@@ -1833,10 +1831,10 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1881,7 +1879,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>⬆ - 6.0</t>
+          <t>⬆ - 13.0</t>
         </is>
       </c>
       <c r="W5" t="n">
@@ -1901,17 +1899,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🔵 1d 7h</t>
+          <t>🔵 1d 5h</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 2h 47m</t>
+          <t>🟢 4h 35m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🟡 15h 4m</t>
+          <t>🟡 15h 18m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1921,54 +1919,54 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 7.28%</t>
+          <t>🟢 6.89%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🟡 6.26%</t>
+          <t>🟡 5.98%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>86.46% - 7.28% - 6.26%</t>
+          <t>87.13% - 6.89% - 5.98%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>92 (58 - 23 - 11)</t>
+          <t>96 (62 - 23 - 11)</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L6" t="n">
+        <v>5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>21</v>
+      </c>
+      <c r="N6" t="n">
         <v>4</v>
       </c>
-      <c r="M6" t="n">
-        <v>22</v>
-      </c>
-      <c r="N6" t="n">
-        <v>3</v>
-      </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬆ - 8h 7m</t>
+          <t>⬆ - 7h 55m</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>⬇ + 13h 55m</t>
+          <t>⬇ + 12h 5m</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>⬆ - 1h 35m</t>
+          <t>⬇ + 13m</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 26m</t>
+          <t>⬇ + 40m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1978,16 +1976,18 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>⬇ + 0.29%</t>
+          <t>⬆ - 0.1%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>⬆ - 9.32%</t>
-        </is>
-      </c>
-      <c r="V6" t="n">
-        <v/>
+          <t>⬆ - 9.6%</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
+        </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
@@ -2003,22 +2003,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🔴 17d 8h</t>
+          <t>🔴 17d</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🟡 2d 5h</t>
+          <t>🟡 1d 21h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🟡 14h 53m</t>
+          <t>🔵 12h 39m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🔴 2d 9h</t>
+          <t>🔴 2d 11h</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2028,54 +2028,54 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🟡 20.68%</t>
+          <t>🟡 15.68%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🟡 5.56%</t>
+          <t>🟡 6.17%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>73.77% - 20.68% - 5.56%</t>
+          <t>78.15% - 15.68% - 6.17%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>70 (51 - 15 - 4)</t>
+          <t>75 (55 - 15 - 5)</t>
         </is>
       </c>
       <c r="K7" t="n">
         <v>35</v>
       </c>
       <c r="L7" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="M7" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" t="n">
         <v>1</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 5d 3h</t>
+          <t>⬇ + 4d 19h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>⬇ + 23h 59m</t>
+          <t>⬇ + 16h 45m</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>⬇ + 9h 26m</t>
+          <t>⬇ + 7h 12m</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>⬇ + 1d 1h</t>
+          <t>⬇ + 1d 2h</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -2085,22 +2085,22 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>⬆ - 2.72%</t>
+          <t>⬆ - 7.72%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>⬇ + 2.88%</t>
+          <t>⬇ + 3.49%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>⬇ + 3.0</t>
+          <t>⬇ + 4.0</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>⬇ + 11.0</t>
+          <t>⬇ + 12.0</t>
         </is>
       </c>
     </row>
@@ -2112,22 +2112,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 8d 16h</t>
+          <t>🟡 8d 15h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 13h 22m</t>
+          <t>🟢 15h 38m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🔵 9h 59m</t>
+          <t>🔵 9h 24m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🔴 1d 10h</t>
+          <t>🔴 1d 7h</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2137,26 +2137,26 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🔵 11.82%</t>
+          <t>🔵 10.56%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🔵 4.6%</t>
+          <t>🔵 4.16%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>83.58% - 11.82% - 4.6%</t>
+          <t>85.29% - 10.56% - 4.16%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>169 (123 - 28 - 18)</t>
+          <t>174 (128 - 28 - 18)</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L8" t="n">
         <v>8</v>
@@ -2169,22 +2169,22 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>⬆ - 5d 10h</t>
+          <t>⬆ - 5d 11h</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 8h 25m</t>
+          <t>⬆ - 6h 9m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 8h 7m</t>
+          <t>⬆ - 8h 42m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>⬆ - 1d 13h</t>
+          <t>⬆ - 1d 15h</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -2194,17 +2194,17 @@
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>⬇ + 3.89%</t>
+          <t>⬇ + 2.63%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>⬆ - 1.07%</t>
+          <t>⬆ - 1.51%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>⬆ - 2.0</t>
+          <t>⬇ + 1.0</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
@@ -2221,22 +2221,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🟡 7d 17h</t>
+          <t>🟡 7d 15h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🟡 2d 22h</t>
+          <t>🟡 2d 15h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🔵 10h 8m</t>
+          <t>🔵 9h 19m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🟡 14h 24m</t>
+          <t>🟡 20h 22m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2246,22 +2246,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 9.61%</t>
+          <t>🔵 9.37%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🔴 7.07%</t>
+          <t>🟡 6.69%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>83.31% - 9.61% - 7.07%</t>
+          <t>83.94% - 9.37% - 6.69%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>42 (30 - 10 - 2)</t>
+          <t>43 (31 - 10 - 2)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -2278,22 +2278,22 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>⬆ - 1d 21h</t>
+          <t>⬆ - 1d 22h</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>⬇ + 18h 47m</t>
+          <t>⬇ + 11h 57m</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>⬇ + 8h 59m</t>
+          <t>⬇ + 8h 10m</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>⬇ + 6h 25m</t>
+          <t>⬇ + 12h 23m</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
@@ -2303,12 +2303,12 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>⬇ + 0.04%</t>
+          <t>⬆ - 0.2%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>⬇ + 4.0%</t>
+          <t>⬇ + 3.62%</t>
         </is>
       </c>
       <c r="V9" t="n">
@@ -2326,105 +2326,101 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 8d</t>
+          <t>🔴 15d 9h</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 5h 25m</t>
+          <t>🟢 5h 28m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 58m</t>
+          <t>🟢 56m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 4h 31m</t>
+          <t>🟢 4h 30m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 7d 13h</t>
+          <t>🔴 14d 22h</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 5.36%</t>
+          <t>🟢 5.6%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 18.74%</t>
+          <t>🔴 19.01%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>75.9% - 5.36% - 18.74%</t>
+          <t>75.39% - 5.6% - 19.01%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>21 (6 - 12 - 3)</t>
+          <t>22 (6 - 13 - 3)</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>⬆ - 2d 19h</t>
+          <t>⬇ + 4d 12h</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>⬆ - 9h 11m</t>
+          <t>⬆ - 9h 8m</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>⬆ - 4h 10m</t>
+          <t>⬆ - 4h 12m</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>⬆ - 2h 15m</t>
+          <t>⬆ - 2h 16m</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>⬆ - 2d 4h</t>
+          <t>⬇ + 5d 4h</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>⬇ + 2.42%</t>
+          <t>⬇ + 2.66%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>⬆ - 3.55%</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>⬇ + 7.0</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>⬇ + 4.0</t>
-        </is>
+          <t>⬆ - 3.28%</t>
+        </is>
+      </c>
+      <c r="V10" t="n">
+        <v/>
+      </c>
+      <c r="W10" t="n">
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -2435,102 +2431,104 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 11d 22h</t>
+          <t>🟡 11d 17h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🔵 1d</t>
+          <t>🔵 23h 52m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🔵 9h 48m</t>
+          <t>🔵 8h 52m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🔴 1d 8h</t>
+          <t>🔴 1d 7h</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🔴 9d 3h</t>
+          <t>🔴 9d 1h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🟡 17.11%</t>
+          <t>🔵 14.29%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🟡 5.72%</t>
+          <t>🟡 5.51%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>77.17% - 17.11% - 5.72%</t>
+          <t>80.2% - 14.29% - 5.51%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>303 (204 - 70 - 29)</t>
+          <t>313 (213 - 70 - 30)</t>
         </is>
       </c>
       <c r="K11" t="n">
         <v>51</v>
       </c>
       <c r="L11" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="M11" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 19h</t>
+          <t>⬇ + 2d 15h</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬇ + 4h 33m</t>
+          <t>⬇ + 3h 33m</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 13m</t>
+          <t>⬆ - 1h 9m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 5h 11m</t>
+          <t>⬆ - 5h 32m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 20h</t>
+          <t>⬇ + 2d 18h</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>⬇ + 5.11%</t>
+          <t>⬇ + 2.29%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>⬆ - 2.46%</t>
-        </is>
-      </c>
-      <c r="V11" t="n">
-        <v/>
+          <t>⬆ - 2.67%</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>⬇ + 5.0</t>
+        </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>⬇ + 12.0</t>
+          <t>⬇ + 13.0</t>
         </is>
       </c>
     </row>
@@ -2542,32 +2540,32 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 9d 9h</t>
+          <t>🟡 11d 20h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🔵 21h 46m</t>
+          <t>🔵 21h 10m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 1h 31m</t>
+          <t>🟢 2h 7m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 11h 38m</t>
+          <t>🔵 11h 42m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 7d 22h</t>
+          <t>🔴 10d 9h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🔵 9.41%</t>
+          <t>🔵 9.36%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -2577,54 +2575,54 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>80.74% - 9.41% - 9.85%</t>
+          <t>80.79% - 9.36% - 9.85%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>140 (81 - 43 - 16)</t>
+          <t>145 (85 - 44 - 16)</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="L12" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M12" t="n">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>⬆ - 19h 25m</t>
+          <t>⬇ + 1d 15h</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>⬇ + 9h 49m</t>
+          <t>⬇ + 9h 13m</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>⬆ - 7h 41m</t>
+          <t>⬆ - 7h 5m</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 1h 52m</t>
+          <t>⬇ + 1h 56m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>⬆ - 23h 25m</t>
+          <t>⬇ + 1d 11h</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>⬇ + 0.22%</t>
+          <t>⬇ + 0.17%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
@@ -2634,12 +2632,12 @@
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>⬇ + 1.0</t>
+          <t>⬆ - 14.0</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>⬇ + 6.0</t>
+          <t>⬇ + 2.0</t>
         </is>
       </c>
     </row>
@@ -2651,22 +2649,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 4d 23h</t>
+          <t>🔵 4d 21h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🟡 2d 3h</t>
+          <t>🟡 1d 23h</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 6h 55m</t>
+          <t>🟢 6h 26m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🟡 15h 48m</t>
+          <t>🟡 18h 46m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -2676,22 +2674,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 6.66%</t>
+          <t>🟢 6.52%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 11.24%</t>
+          <t>🔴 11.08%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>82.1% - 6.66% - 11.24%</t>
+          <t>82.4% - 6.52% - 11.08%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>58 (42 - 14 - 2)</t>
+          <t>60 (43 - 15 - 2)</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -2708,22 +2706,22 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>⬆ - 13h 47m</t>
+          <t>⬆ - 15h 18m</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>⬇ + 17h 31m</t>
+          <t>⬇ + 13h 31m</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>⬇ + 3h 46m</t>
+          <t>⬇ + 3h 17m</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>⬇ + 4h 33m</t>
+          <t>⬇ + 7h 31m</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
@@ -2733,12 +2731,12 @@
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>⬆ - 0.28%</t>
+          <t>⬆ - 0.42%</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>⬆ - 11.14%</t>
+          <t>⬆ - 11.3%</t>
         </is>
       </c>
       <c r="V13" t="n">
@@ -2756,103 +2754,103 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>🟡 9d 20h</t>
+          <t>🟡 9d 6h</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🟢 17h 14m</t>
+          <t>🟢 15h 44m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🟢 5h 14m</t>
+          <t>🟢 5h 43m</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>🟡 15h 59m</t>
+          <t>🔵 13h 49m</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>🔴 8d 6h</t>
+          <t>🔴 7d 19h</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>🔵 9.35%</t>
+          <t>🔵 9.82%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>🔴 22.59%</t>
+          <t>🔴 22.08%</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>68.06% - 9.35% - 22.59%</t>
+          <t>68.1% - 9.82% - 22.08%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>38 (17 - 12 - 9)</t>
+          <t>39 (18 - 12 - 9)</t>
         </is>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
         <v>0</v>
       </c>
       <c r="M14" t="n">
+        <v>2</v>
+      </c>
+      <c r="N14" t="n">
         <v>1</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>⬇ + 1d 19h</t>
+          <t>⬇ + 1d 5h</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>⬇ + 7h 4m</t>
+          <t>⬇ + 5h 34m</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>⬆ - 1d 10h</t>
+          <t>⬆ - 1d 9h</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>⬆ - 1d 10h</t>
+          <t>⬆ - 1d 12h</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>⬇ + 4d 9h</t>
+          <t>⬇ + 3d 21h</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>⬆ - 13.68%</t>
+          <t>⬆ - 13.21%</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>⬇ + 18.46%</t>
-        </is>
-      </c>
-      <c r="V14" t="n">
+          <t>⬇ + 17.95%</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>⬇ + 1.0</t>
+        </is>
+      </c>
+      <c r="W14" t="n">
         <v/>
-      </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>⬆ - 1.0</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajuste de posicionamento do template add comparativo nas posicoes abaixo
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -847,17 +847,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 23.4%</t>
+          <t>🔴 23.75%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🔵 2.68%</t>
+          <t>🔵 2.72%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>73.92% - 23.4% - 2.68%</t>
+          <t>73.53% - 23.75% - 2.72%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 9d 18h</t>
+          <t>🟡 12d 6h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🔴 6d 14h</t>
+          <t>🔴 9d 2h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🔵 6d 8h</t>
+          <t>🟡 8d 8h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>🟡 4d 14h</t>
+          <t>🔴 6d 13h</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🔵 6d 4h</t>
+          <t>🟡 7d</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1098,22 +1098,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🟡 4d 5h</t>
+          <t>🟡 5d 1h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🔵 12.0%</t>
+          <t>🔵 12.11%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🔴 8.18%</t>
+          <t>🔴 8.2%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>79.82% - 12.0% - 8.18%</t>
+          <t>79.69% - 12.11% - 8.2%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 3d 16h</t>
+          <t>🔵 4d 16h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>🟡 2d 7h</t>
+          <t>🟡 3d 6h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1337,7 +1337,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1461,6 +1461,11 @@
           <t>dt_total_diff</t>
         </is>
       </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>total_release_deploy_diff</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1470,22 +1475,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 1d 14h</t>
+          <t>🟢 1d 13h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🔵 21h 25m</t>
+          <t>🔵 19h 44m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 2h 33m</t>
+          <t>🟢 2h 25m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🟡 14h 17m</t>
+          <t>🟡 15h 1m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -1495,17 +1500,17 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 3.42%</t>
+          <t>🟢 3.51%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 16.25%</t>
+          <t>🔴 15.47%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>80.33% - 3.42% - 16.25%</t>
+          <t>81.02% - 3.51% - 15.47%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1527,22 +1532,22 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>⬇ + 13h 24m</t>
+          <t>⬇ + 12h 19m</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>⬇ + 11h 48m</t>
+          <t>⬇ + 10h 7m</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>⬆ - 1h 51m</t>
+          <t>⬆ - 1h 59m</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>⬇ + 3h 27m</t>
+          <t>⬇ + 4h 11m</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -1552,19 +1557,28 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>⬆ - 0.91%</t>
+          <t>⬆ - 0.82%</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>⬆ - 26.08%</t>
-        </is>
-      </c>
-      <c r="V2" t="n">
-        <v/>
-      </c>
-      <c r="W2" t="n">
-        <v/>
+          <t>⬆ - 26.86%</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1575,22 +1589,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🟡 6d 13h</t>
+          <t>🟡 6d 14h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 11h 17m</t>
+          <t>🟢 11h 53m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🟢 4h 14m</t>
+          <t>🟢 4h 1m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🔵 11h 21m</t>
+          <t>🔵 12h 8m</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1600,17 +1614,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🔵 9.82%</t>
+          <t>🔵 9.59%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>🔴 22.07%</t>
+          <t>🔴 22.32%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>68.12% - 9.82% - 22.07%</t>
+          <t>68.09% - 9.59% - 22.32%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1632,22 +1646,22 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>⬇ + 18h 31m</t>
+          <t>⬇ + 19h 41m</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>⬇ + 3h 52m</t>
+          <t>⬇ + 4h 28m</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>⬆ - 22h 7m</t>
+          <t>⬆ - 22h 20m</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>⬆ - 22h 39m</t>
+          <t>⬆ - 21h 52m</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -1657,12 +1671,12 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>⬆ - 13.21%</t>
+          <t>⬆ - 13.44%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>⬇ + 17.94%</t>
+          <t>⬇ + 18.19%</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -1670,8 +1684,15 @@
           <t>⬇ + 1.0</t>
         </is>
       </c>
-      <c r="W3" t="n">
-        <v/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>⬆ - 2.0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -1682,42 +1703,42 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟡 6d 12h</t>
+          <t>🟡 9d 5h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 6h 25m</t>
+          <t>🟢 5h 59m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 3h 53m</t>
+          <t>🟢 3h 51m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🟢 2h 33m</t>
+          <t>🟢 2h 38m</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>🔴 5d 23h</t>
+          <t>🔴 8d 17h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🟡 15.04%</t>
+          <t>🔵 14.75%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🟡 5.94%</t>
+          <t>🟡 6.3%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>79.02% - 15.04% - 5.94%</t>
+          <t>78.95% - 14.75% - 6.3%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -1739,44 +1760,53 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>⬇ + 5d 18h</t>
+          <t>⬇ + 8d 12h</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>⬆ - 28m</t>
+          <t>⬆ - 54m</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>⬆ - 38m</t>
+          <t>⬆ - 40m</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>⬆ - 3h 35m</t>
+          <t>⬆ - 3h 30m</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>⬇ + 5d 23h</t>
+          <t>⬇ + 8d 17h</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>⬇ + 10.38%</t>
+          <t>⬇ + 10.09%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>⬆ - 10.26%</t>
-        </is>
-      </c>
-      <c r="V4" t="n">
-        <v/>
-      </c>
-      <c r="W4" t="n">
-        <v/>
+          <t>⬆ - 9.9%</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>⬆ - 7.0</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -1787,42 +1817,42 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>🔴 14d 7h</t>
+          <t>🔴 15d 17h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>🔵 19h 49m</t>
+          <t>🔵 1d</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🟢 50m</t>
+          <t>🟢 57m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🔵 8h 28m</t>
+          <t>🔵 9h 52m</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>🔴 13d 2h</t>
+          <t>🔴 14d 6h</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🟡 16.0%</t>
+          <t>🟡 15.63%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🟡 5.25%</t>
+          <t>🟡 5.03%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>78.75% - 16.0% - 5.25%</t>
+          <t>79.34% - 15.63% - 5.03%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -1844,37 +1874,37 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>⬇ + 5d 16h</t>
+          <t>⬇ + 7d 1h</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>⬇ + 17h 25m</t>
+          <t>⬇ + 21h 36m</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>⬆ - 9h 59m</t>
+          <t>⬆ - 9h 52m</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>⬇ + 1h 59m</t>
+          <t>⬇ + 3h 23m</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>⬇ + 5d 7h</t>
+          <t>⬇ + 6d 10h</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>⬆ - 1.64%</t>
+          <t>⬆ - 2.01%</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>⬇ + 3.03%</t>
+          <t>⬇ + 2.81%</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1882,8 +1912,15 @@
           <t>⬆ - 13.0</t>
         </is>
       </c>
-      <c r="W5" t="n">
-        <v/>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>⬇ + 4.0</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -1899,17 +1936,17 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🔵 21h 32m</t>
+          <t>🔵 23h 21m</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 4h 3m</t>
+          <t>🟢 3h 7m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 10h 56m</t>
+          <t>🔵 10h 44m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1919,17 +1956,17 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 6.89%</t>
+          <t>🟢 7.41%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🟡 5.98%</t>
+          <t>🟡 6.45%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>87.13% - 6.89% - 5.98%</t>
+          <t>86.15% - 7.41% - 6.45%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -1951,22 +1988,22 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬇ + 31m</t>
+          <t>⬇ + 1h 12m</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>⬇ + 7h 34m</t>
+          <t>⬇ + 9h 23m</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>⬇ + 23m</t>
+          <t>⬆ - 33m</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 48m</t>
+          <t>⬇ + 1h 36m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -1976,12 +2013,12 @@
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>⬆ - 0.1%</t>
+          <t>⬇ + 0.42%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>⬆ - 9.6%</t>
+          <t>⬆ - 9.13%</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -1992,6 +2029,11 @@
       <c r="W6" t="inlineStr">
         <is>
           <t>⬇ + 2.0</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>⬆ - 1.0</t>
         </is>
       </c>
     </row>
@@ -2003,22 +2045,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 12d 6h</t>
+          <t>🟡 11d 14h</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🔵 1d 10h</t>
+          <t>🔵 1d 2h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🔵 8h 54m</t>
+          <t>🔵 7h 22m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🔴 1d 19h</t>
+          <t>🔴 1d 13h</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -2028,17 +2070,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🟡 18.35%</t>
+          <t>🔴 21.45%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🔵 4.89%</t>
+          <t>🟡 5.41%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>76.76% - 18.35% - 4.89%</t>
+          <t>73.14% - 21.45% - 5.41%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -2060,22 +2102,22 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 4d 3h</t>
+          <t>⬇ + 3d 12h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>⬇ + 12h 55m</t>
+          <t>⬇ + 4h 43m</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>⬇ + 4h 6m</t>
+          <t>⬇ + 2h 34m</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>⬇ + 20h 10m</t>
+          <t>⬇ + 14h 4m</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
@@ -2085,12 +2127,12 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>⬆ - 5.05%</t>
+          <t>⬆ - 2.3%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>⬇ + 2.21%</t>
+          <t>⬇ + 2.69%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
@@ -2101,6 +2143,11 @@
       <c r="W7" t="inlineStr">
         <is>
           <t>⬇ + 12.0</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2112,42 +2159,42 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🔵 6d 5h</t>
+          <t>🟡 6d 17h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 10h 22m</t>
+          <t>🟢 10h 19m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🟢 5h 32m</t>
+          <t>🟢 6h</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🟡 22h 39m</t>
+          <t>🟡 23h 32m</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🟡 4d 15h</t>
+          <t>🟡 5d 1h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🔵 10.46%</t>
+          <t>🔵 11.11%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🔵 4.11%</t>
+          <t>🔵 4.32%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>85.44% - 10.46% - 4.11%</t>
+          <t>84.57% - 11.11% - 4.32%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -2169,17 +2216,17 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>⬆ - 3d 12h</t>
+          <t>⬆ - 5d 13h</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 13m</t>
+          <t>⬆ - 5h 16m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 6h 15m</t>
+          <t>⬆ - 5h 47m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
@@ -2189,17 +2236,17 @@
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>⬆ - 1d 23h</t>
+          <t>⬆ - 4d 1h</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>⬇ + 2.53%</t>
+          <t>⬇ + 3.18%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>⬆ - 1.56%</t>
+          <t>⬆ - 1.35%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
@@ -2210,6 +2257,11 @@
       <c r="W8" t="inlineStr">
         <is>
           <t>⬇ + 1.0</t>
+        </is>
+      </c>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>⬇ + 9.0</t>
         </is>
       </c>
     </row>
@@ -2221,22 +2273,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🔵 5d 13h</t>
+          <t>🔵 5d 12h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🔵 1d 18h</t>
+          <t>🔵 1d 19h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🔵 7h 1m</t>
+          <t>🟢 5h 14m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🟡 15h 12m</t>
+          <t>🟡 14h 27m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2246,17 +2298,17 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 9.11%</t>
+          <t>🔵 9.06%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🟡 6.81%</t>
+          <t>🟡 6.66%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>84.09% - 9.11% - 6.81%</t>
+          <t>84.29% - 9.06% - 6.66%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -2278,44 +2330,53 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>⬆ - 19h 29m</t>
+          <t>⬆ - 2d 20h</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>⬇ + 7h 13m</t>
+          <t>⬇ + 8h 41m</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>⬇ + 5h 52m</t>
+          <t>⬇ + 4h 5m</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>⬇ + 8h 29m</t>
+          <t>⬇ + 7h 44m</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>⬆ - 1d 17h</t>
+          <t>⬆ - 3d 16h</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>⬆ - 0.46%</t>
+          <t>⬆ - 0.51%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>⬇ + 3.74%</t>
-        </is>
-      </c>
-      <c r="V9" t="n">
-        <v/>
-      </c>
-      <c r="W9" t="n">
-        <v/>
+          <t>⬇ + 3.59%</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>⬇ + 3.0</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -2326,42 +2387,42 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 10d 18h</t>
+          <t>🟡 11d 5h</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>🟢 4h 1m</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>🟢 32m</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>🟢 3h 43m</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>🟢 30m</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>🟢 3h 39m</t>
-        </is>
-      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 10d 10h</t>
+          <t>🔴 10d 21h</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 5.47%</t>
+          <t>🟢 4.22%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 19.0%</t>
+          <t>🔴 18.65%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>75.53% - 5.47% - 19.0%</t>
+          <t>77.13% - 4.22% - 18.65%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -2383,44 +2444,53 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>⬇ + 3d 8h</t>
+          <t>⬇ + 3d 19h</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>⬆ - 6h 13m</t>
+          <t>⬆ - 5h 55m</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>⬆ - 3h 18m</t>
+          <t>⬆ - 3h 16m</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>⬆ - 1h 8m</t>
+          <t>⬆ - 1h 4m</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>⬇ + 3d 18h</t>
+          <t>⬇ + 4d 5h</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>⬇ + 2.53%</t>
+          <t>⬇ + 1.28%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>⬆ - 3.29%</t>
-        </is>
-      </c>
-      <c r="V10" t="n">
-        <v/>
-      </c>
-      <c r="W10" t="n">
-        <v/>
+          <t>⬆ - 3.64%</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -2431,42 +2501,42 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 8d 8h</t>
+          <t>🟡 9d 4h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 17h</t>
+          <t>🟢 14h 6m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🟢 6h 6m</t>
+          <t>🟢 5h 44m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 23h 1m</t>
+          <t>🟡 21h 19m</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🔴 6d 9h</t>
+          <t>🔴 7d 11h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🔵 14.62%</t>
+          <t>🟡 15.77%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🔵 4.97%</t>
+          <t>🟡 5.34%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>80.41% - 14.62% - 4.97%</t>
+          <t>78.89% - 15.77% - 5.34%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -2493,32 +2563,32 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬇ + 2h 25m</t>
+          <t>⬆ - 29m</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 56m</t>
+          <t>⬆ - 1h 18m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 3h 7m</t>
+          <t>⬆ - 4h 49m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 4h</t>
+          <t>⬇ + 2d 10h</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>⬇ + 2.62%</t>
+          <t>⬇ + 3.66%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>⬆ - 3.21%</t>
+          <t>⬆ - 2.86%</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
@@ -2529,6 +2599,11 @@
       <c r="W11" t="inlineStr">
         <is>
           <t>⬇ + 13.0</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2540,42 +2615,42 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 9d 22h</t>
+          <t>🟡 10d 13h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🟢 15h 1m</t>
+          <t>🟢 17h 7m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 1h 47m</t>
+          <t>🟢 1h 32m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 7h 41m</t>
+          <t>🔵 8h 6m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 8d 22h</t>
+          <t>🔴 9d 11h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🔵 9.45%</t>
+          <t>🔵 9.09%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 10.08%</t>
+          <t>🔴 10.04%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>80.47% - 9.45% - 10.08%</t>
+          <t>80.87% - 9.09% - 10.04%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -2597,37 +2672,37 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>⬇ + 3d</t>
+          <t>⬇ + 3d 15h</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>⬇ + 6h 15m</t>
+          <t>⬇ + 8h 21m</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>⬆ - 4h 18m</t>
+          <t>⬆ - 4h 33m</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 53m</t>
+          <t>⬇ + 1h 18m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>⬇ + 2d 21h</t>
+          <t>⬇ + 3d 10h</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>⬇ + 0.26%</t>
+          <t>⬆ - 0.1%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>⬆ - 3.28%</t>
+          <t>⬆ - 3.32%</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
@@ -2638,6 +2713,11 @@
       <c r="W12" t="inlineStr">
         <is>
           <t>⬇ + 2.0</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2649,7 +2729,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 3d 13h</t>
+          <t>🔵 3d 12h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2659,7 +2739,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 4h 47m</t>
+          <t>🟢 3h 49m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -2674,17 +2754,17 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 6.26%</t>
+          <t>🟢 6.28%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 11.53%</t>
+          <t>🔴 11.06%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>82.21% - 6.26% - 11.53%</t>
+          <t>82.66% - 6.28% - 11.06%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -2706,17 +2786,17 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>⬆ - 3h 3m</t>
+          <t>⬆ - 1d 3h</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>⬇ + 9h 31m</t>
+          <t>⬇ + 9h 24m</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>⬇ + 2h 1m</t>
+          <t>⬇ + 1h 3m</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -2726,24 +2806,33 @@
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>⬆ - 20h 31m</t>
+          <t>⬆ - 1d 20h</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>⬆ - 0.69%</t>
+          <t>⬆ - 0.67%</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>⬆ - 11.16%</t>
-        </is>
-      </c>
-      <c r="V13" t="n">
-        <v/>
-      </c>
-      <c r="W13" t="n">
-        <v/>
+          <t>⬆ - 11.63%</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -2754,22 +2843,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>🟡 6d 13h</t>
+          <t>🟡 6d 14h</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🟢 11h 17m</t>
+          <t>🟢 11h 53m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🟢 4h 14m</t>
+          <t>🟢 4h 1m</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>🔵 11h 21m</t>
+          <t>🔵 12h 8m</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2779,17 +2868,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>🔵 9.82%</t>
+          <t>🔵 9.59%</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>🔴 22.06%</t>
+          <t>🔴 22.32%</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>68.12% - 9.82% - 22.06%</t>
+          <t>68.09% - 9.59% - 22.32%</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -2811,22 +2900,22 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>⬇ + 18h 31m</t>
+          <t>⬇ + 19h 41m</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>⬇ + 3h 52m</t>
+          <t>⬇ + 4h 28m</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>⬆ - 22h 7m</t>
+          <t>⬆ - 22h 20m</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>⬆ - 22h 39m</t>
+          <t>⬆ - 21h 52m</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -2836,12 +2925,12 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>⬆ - 13.21%</t>
+          <t>⬆ - 13.44%</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>⬇ + 17.93%</t>
+          <t>⬇ + 18.19%</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
@@ -2849,8 +2938,15 @@
           <t>⬇ + 1.0</t>
         </is>
       </c>
-      <c r="W14" t="n">
-        <v/>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criado um novo template "informe lideres" que avalia os dados de cada colaborador tech do time
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -1594,12 +1594,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 11h 53m</t>
+          <t>🟢 12h 14m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🟢 4h 1m</t>
+          <t>🟢 4h 8m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1646,17 +1646,17 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>⬇ + 19h 41m</t>
+          <t>⬇ + 20h 9m</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>⬇ + 4h 28m</t>
+          <t>⬇ + 4h 49m</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>⬆ - 22h 20m</t>
+          <t>⬆ - 22h 13m</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>⬆ - 2.0</t>
+          <t>⬆ + 2.0</t>
         </is>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>⬆ - 7.0</t>
+          <t>⬆ + 7.0</t>
         </is>
       </c>
     </row>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>⬇ + 4.0</t>
+          <t>⬇ - 4.0</t>
         </is>
       </c>
     </row>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🔵 4d 18h</t>
+          <t>🔵 4d 19h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 10h 44m</t>
+          <t>🔵 11h 37m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -1988,7 +1988,7 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 12m</t>
+          <t>⬇ + 2h 5m</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 36m</t>
+          <t>⬇ + 2h 29m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>⬆ - 1.0</t>
+          <t>⬆ + 1.0</t>
         </is>
       </c>
     </row>
@@ -2045,7 +2045,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 11d 14h</t>
+          <t>🟡 11d 15h</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2065,7 +2065,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>🔴 8d 15h</t>
+          <t>🔴 8d 16h</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 3d 12h</t>
+          <t>⬇ + 3d 13h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>⬇ + 2d 14h</t>
+          <t>⬇ + 2d 16h</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -2164,17 +2164,17 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 10h 19m</t>
+          <t>🟢 10h 27m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🟢 6h</t>
+          <t>🟢 5h 58m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🟡 23h 32m</t>
+          <t>🟡 23h 40m</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -2221,17 +2221,17 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 16m</t>
+          <t>⬆ - 5h 8m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 47m</t>
+          <t>⬆ - 5h 49m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>⬆ - 1d 1h</t>
+          <t>⬆ - 1d</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>⬇ + 9.0</t>
+          <t>⬇ - 9.0</t>
         </is>
       </c>
     </row>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>⬇ + 3.0</t>
+          <t>⬇ - 3.0</t>
         </is>
       </c>
     </row>
@@ -2506,17 +2506,17 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 14h 6m</t>
+          <t>🟢 14h 9m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🟢 5h 44m</t>
+          <t>🟢 5h 43m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 21h 19m</t>
+          <t>🟡 21h 21m</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -2558,22 +2558,22 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 3h</t>
+          <t>⬇ + 2d 4h</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬆ - 29m</t>
+          <t>⬆ - 26m</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 1h 18m</t>
+          <t>⬆ - 1h 19m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 4h 49m</t>
+          <t>⬆ - 4h 47m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 10d 13h</t>
+          <t>🟡 10d 14h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 8h 6m</t>
+          <t>🔵 8h 24m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 1h 18m</t>
+          <t>⬇ + 1h 36m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -2848,12 +2848,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🟢 11h 53m</t>
+          <t>🟢 12h 14m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🟢 4h 1m</t>
+          <t>🟢 4h 8m</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -2900,17 +2900,17 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>⬇ + 19h 41m</t>
+          <t>⬇ + 20h 9m</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>⬇ + 4h 28m</t>
+          <t>⬇ + 4h 49m</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>⬆ - 22h 20m</t>
+          <t>⬆ - 22h 13m</t>
         </is>
       </c>
       <c r="R14" t="inlineStr">

</xml_diff>

<commit_message>
add new service: owner_ticketing
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Octubre" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Noviembre" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Noviembre" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Diciembre" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,22 +502,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 1d</t>
+          <t>🟢 1d 13h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🟢 9h 37m</t>
+          <t>🔵 19h 44m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 4h 24m</t>
+          <t>🟢 2h 25m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🔵 10h 50m</t>
+          <t>🟡 15h 1m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -527,22 +527,22 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 4.33%</t>
+          <t>🟢 3.51%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 42.33%</t>
+          <t>🔴 15.49%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>53.34% - 4.33% - 42.33%</t>
+          <t>81.0% - 3.51% - 15.49%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>25 (18 - 7 - 0)</t>
+          <t>17 (12 - 5 - 0)</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -566,60 +566,60 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🔵 5d 18h</t>
+          <t>🟡 6d 14h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 7h 25m</t>
+          <t>🟢 12h 14m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🔴 1d 2h</t>
+          <t>🟢 4h 8m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🔴 1d 10h</t>
+          <t>🔵 12h 8m</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>🟡 2d 22h</t>
+          <t>🟡 5d 10h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🔴 23.03%</t>
+          <t>🔵 9.59%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>🔵 4.13%</t>
+          <t>🔴 22.32%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>72.84% - 23.03% - 4.13%</t>
+          <t>68.09% - 9.59% - 22.32%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>31 (16 - 8 - 7)</t>
+          <t>39 (18 - 12 - 9)</t>
         </is>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -630,54 +630,54 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟢 17h 32m</t>
+          <t>🟡 9d 5h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 6h 53m</t>
+          <t>🟢 6h 26m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 4h 31m</t>
+          <t>🟢 3h 51m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🔵 6h 8m</t>
+          <t>🟢 2h 38m</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>⚪ 0m</t>
+          <t>🔴 8d 17h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🟢 4.66%</t>
+          <t>🔵 14.75%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🔴 16.2%</t>
+          <t>🟡 6.3%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>79.14% - 4.66% - 16.2%</t>
+          <t>78.95% - 14.75% - 6.3%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>34 (34 - 0 - 0)</t>
+          <t>64 (30 - 27 - 7)</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
@@ -694,54 +694,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>🟡 8d 15h</t>
+          <t>🔴 15d 17h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>🟢 2h 24m</t>
+          <t>🔵 1d</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🔵 10h 49m</t>
+          <t>🟢 57m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🔵 6h 29m</t>
+          <t>🔵 9h 52m</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>🔴 7d 19h</t>
+          <t>🔴 14d 6h</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🟡 17.64%</t>
+          <t>🟡 15.63%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🔵 2.22%</t>
+          <t>🟡 5.03%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>80.15% - 17.64% - 2.22%</t>
+          <t>79.34% - 15.63% - 5.03%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>52 (29 - 17 - 6)</t>
+          <t>27 (17 - 8 - 2)</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="L5" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -758,60 +758,60 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🔵 4d 17h</t>
+          <t>🔵 4d 19h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🟢 13h 58m</t>
+          <t>🔵 23h 21m</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 3h 40m</t>
+          <t>🟢 3h 7m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 9h 8m</t>
+          <t>🔵 11h 37m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>🟡 3d 14h</t>
+          <t>🟡 3d 5h</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 6.99%</t>
+          <t>🟢 7.41%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🔴 15.58%</t>
+          <t>🟡 6.45%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>77.44% - 6.99% - 15.58%</t>
+          <t>86.15% - 7.41% - 6.45%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>109 (65 - 34 - 10)</t>
+          <t>96 (62 - 23 - 11)</t>
         </is>
       </c>
       <c r="K6" t="n">
         <v>9</v>
       </c>
       <c r="L6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="M6" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N6" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -822,60 +822,60 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 8d 2h</t>
+          <t>🟡 11d 15h</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🔵 21h 18m</t>
+          <t>🔵 1d 2h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🟢 4h 48m</t>
+          <t>🔵 7h 22m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🟡 23h 43m</t>
+          <t>🔴 1d 13h</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>🔴 6d</t>
+          <t>🔴 8d 16h</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 23.75%</t>
+          <t>🔴 21.45%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🔵 2.72%</t>
+          <t>🟡 5.41%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>73.53% - 23.75% - 2.72%</t>
+          <t>73.14% - 21.45% - 5.41%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>90 (56 - 29 - 5)</t>
+          <t>75 (55 - 15 - 5)</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="L7" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="M7" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="N7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -886,57 +886,57 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 12d 6h</t>
+          <t>🟡 6d 17h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 15h 35m</t>
+          <t>🟢 10h 20m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🔵 11h 47m</t>
+          <t>🟢 6h 4m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🔴 2d</t>
+          <t>🟡 23h 40m</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🔴 9d 2h</t>
+          <t>🟡 5d 1h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🟢 7.93%</t>
+          <t>🟢 8.88%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🟡 5.67%</t>
+          <t>🔵 3.53%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>86.4% - 7.93% - 5.67%</t>
+          <t>87.59% - 8.88% - 3.53%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>173 (112 - 34 - 27)</t>
+          <t>143 (103 - 24 - 16)</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L8" t="n">
+        <v>8</v>
+      </c>
+      <c r="M8" t="n">
         <v>1</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
       </c>
       <c r="N8" t="n">
         <v>0</v>
@@ -950,47 +950,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🟡 8d 8h</t>
+          <t>🔵 5d 12h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🔵 1d 10h</t>
+          <t>🔵 1d 19h</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🟢 1h 9m</t>
+          <t>🟢 5h 14m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🔵 6h 43m</t>
+          <t>🟡 14h 27m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>🔴 6d 13h</t>
+          <t>🟡 2d 20h</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 9.57%</t>
+          <t>🔵 9.06%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🔵 3.07%</t>
+          <t>🟡 6.66%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>87.37% - 9.57% - 3.07%</t>
+          <t>84.29% - 9.06% - 6.66%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>42 (29 - 8 - 5)</t>
+          <t>43 (31 - 10 - 2)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -1009,62 +1009,62 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>owner_tipodecambio</t>
+          <t>owner_ticketing</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 7d 10h</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 9h 56m</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 3h 48m</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 4h 47m</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 6d 15h</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 2.94%</t>
+          <t>🟢 7.89%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 22.29%</t>
+          <t>🟢 1.68%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>74.76% - 2.94% - 22.29%</t>
+          <t>90.43% - 7.89% - 1.68%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>40 (29 - 8 - 3)</t>
+          <t>35 (27 - 6 - 2)</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L10" t="n">
         <v>0</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10" t="n">
         <v>0</v>
@@ -1073,257 +1073,321 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>retail</t>
+          <t>owner_tipodecambio</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 7d</t>
+          <t>🟡 11d 5h</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 14h 35m</t>
+          <t>🟢 4h 1m</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🔵 7h 2m</t>
+          <t>🟢 32m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 1d 2h</t>
+          <t>🟢 3h 43m</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🟡 5d 1h</t>
+          <t>🔴 10d 21h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🔵 12.11%</t>
+          <t>🟢 4.21%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🔴 8.2%</t>
+          <t>🔴 18.63%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>79.69% - 12.11% - 8.2%</t>
+          <t>77.16% - 4.21% - 18.63%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>297 (202 - 63 - 32)</t>
+          <t>22 (6 - 13 - 3)</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="L11" t="n">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="M11" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="N11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>financial</t>
+          <t>retail</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 6d 22h</t>
+          <t>🟡 6d 21h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🟢 8h 46m</t>
+          <t>🟢 10h 41m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 6h 5m</t>
+          <t>🟢 4h 19m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 6h 48m</t>
+          <t>🟡 16h 1m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 6d</t>
+          <t>🟡 5d 14h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🔵 9.19%</t>
+          <t>🔵 13.24%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 13.36%</t>
+          <t>🔵 4.23%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>77.45% - 9.19% - 13.36%</t>
+          <t>82.53% - 13.24% - 4.23%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>201 (123 - 59 - 19)</t>
+          <t>317 (215 - 72 - 30)</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="L12" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M12" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N12" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>negocios</t>
+          <t>financial</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 4d 16h</t>
+          <t>🟡 10d 14h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🔵 22h 15m</t>
+          <t>🟢 17h 7m</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 2h 46m</t>
+          <t>🟢 1h 32m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🔵 8h 46m</t>
+          <t>🔵 8h 24m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>🟡 3d 6h</t>
+          <t>🔴 9d 11h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 6.95%</t>
+          <t>🔵 9.08%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 22.69%</t>
+          <t>🔴 10.04%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>70.36% - 6.95% - 22.69%</t>
+          <t>80.88% - 9.08% - 10.04%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>67 (47 - 15 - 5)</t>
+          <t>145 (85 - 44 - 16)</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>negocios</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>🔵 3d 12h</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>🔵 1d 7h</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>🟢 3h 49m</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>🟡 14h 44m</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>🔵 1d 10h</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>🟢 6.28%</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>🔴 11.07%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>82.65% - 6.28% - 11.07%</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>60 (43 - 15 - 2)</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>product cx</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>🔵 5d 18h</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>🟢 7h 25m</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>🔴 1d 2h</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>🔴 1d 10h</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>🟡 2d 22h</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>🔴 23.03%</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>🔵 4.13%</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>72.84% - 23.03% - 4.13%</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>31 (16 - 8 - 7)</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>2</v>
-      </c>
-      <c r="N14" t="n">
-        <v>2</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>🟡 6d 14h</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>🟢 12h 14m</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>🟢 4h 8m</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>🔵 12h 8m</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>🟡 5d 10h</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>🔵 9.59%</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>🔴 22.32%</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>68.09% - 9.59% - 22.32%</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>39 (18 - 12 - 9)</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1337,7 +1401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1475,47 +1539,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>🟢 1d 13h</t>
+          <t>🟡 12d 15h</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>🔵 19h 44m</t>
+          <t>🟢 4h 46m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🟢 2h 25m</t>
+          <t>🟢 1h 47m</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🟡 15h 1m</t>
+          <t>🔵 13h 28m</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>⚪ 0m</t>
+          <t>🔴 11d 19h</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>🟢 3.51%</t>
+          <t>🔴 28.03%</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>🔴 15.47%</t>
+          <t>🔴 7.71%</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>81.02% - 3.51% - 15.47%</t>
+          <t>64.26% - 28.03% - 7.71%</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>17 (12 - 5 - 0)</t>
+          <t>11 (2 - 4 - 5)</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -1532,52 +1596,52 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>⬇ + 12h 19m</t>
+          <t>⬇ + 11d 2h</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>⬇ + 10h 7m</t>
+          <t>⬆ - 14h 58m</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>⬆ - 1h 59m</t>
+          <t>⬆ - 38m</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>⬇ + 4h 11m</t>
+          <t>⬆ - 1h 33m</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
+          <t>⬇ + 11d 19h</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>⬇ + 24.52%</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>⬆ - 7.78%</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>⬆ - 0.82%</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>⬆ - 26.86%</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬆ + 5.0</t>
         </is>
       </c>
     </row>
@@ -1589,109 +1653,109 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>🟡 6d 14h</t>
+          <t>🔵 3d 17h</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>🟢 11h 53m</t>
+          <t>🟢 11h 12m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🟢 4h 1m</t>
+          <t>🟡 16h 17m</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>🔵 12h 8m</t>
+          <t>🔵 10h 44m</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>🟡 5d 10h</t>
+          <t>🟡 2d 3h</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>🔵 9.59%</t>
+          <t>🔴 34.73%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>🔴 22.32%</t>
+          <t>🔵 4.2%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>68.09% - 9.59% - 22.32%</t>
+          <t>61.06% - 34.73% - 4.2%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>39 (18 - 12 - 9)</t>
+          <t>16 (8 - 5 - 3)</t>
         </is>
       </c>
       <c r="K3" t="n">
         <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N3" t="n">
         <v>1</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>⬇ + 19h 41m</t>
+          <t>⬆ - 2d 21h</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>⬇ + 4h 28m</t>
+          <t>⬆ - 1h 2m</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>⬆ - 22h 20m</t>
+          <t>⬇ + 12h 9m</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>⬆ - 21h 52m</t>
+          <t>⬆ - 1h 24m</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>⬇ + 2d 11h</t>
+          <t>⬆ - 3d 7h</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>⬆ - 13.44%</t>
+          <t>⬇ + 25.14%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>⬇ + 18.19%</t>
+          <t>⬆ - 18.12%</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>⬇ + 1.0</t>
+          <t>=</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬇ + 3.0</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>⬆ - 2.0</t>
+          <t>⬇ - 6.0</t>
         </is>
       </c>
     </row>
@@ -1703,51 +1767,51 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>🟡 9d 5h</t>
+          <t>🔵 3d 14h</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>🟢 5h 59m</t>
+          <t>🟢 14h 3m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🟢 3h 51m</t>
+          <t>🟢 2h 34m</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>🟢 2h 38m</t>
+          <t>🔴 1d 17h</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>🔴 8d 17h</t>
+          <t>🔵 1d 4h</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>🔵 14.75%</t>
+          <t>🟡 20.55%</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>🟡 6.3%</t>
+          <t>🔴 7.27%</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>78.95% - 14.75% - 6.3%</t>
+          <t>72.18% - 20.55% - 7.27%</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>64 (30 - 27 - 7)</t>
+          <t>32 (15 - 11 - 6)</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
@@ -1760,52 +1824,52 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>⬇ + 8d 12h</t>
+          <t>⬆ - 5d 15h</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>⬆ - 54m</t>
+          <t>⬇ + 7h 37m</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>⬆ - 40m</t>
+          <t>⬆ - 1h 17m</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>⬆ - 3h 30m</t>
+          <t>⬇ + 1d 15h</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>⬇ + 8d 17h</t>
+          <t>⬆ - 7d 12h</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>⬇ + 10.09%</t>
+          <t>⬇ + 5.8%</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>⬆ - 9.9%</t>
+          <t>⬇ + 0.97%</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
+          <t>⬇ + 6.0</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>⬆ - 7.0</t>
+          <t>⬇ - 1.0</t>
         </is>
       </c>
     </row>
@@ -1817,54 +1881,54 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>🔴 15d 17h</t>
+          <t>🔵 4d 1h</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>🔵 1d</t>
+          <t>🟢 7h 18m</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🟢 57m</t>
+          <t>🟢 2h 48m</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>🔵 9h 52m</t>
+          <t>🔴 1d 20h</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>🔴 14d 6h</t>
+          <t>🔵 1d 19h</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>🟡 15.63%</t>
+          <t>🟢 2.12%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>🟡 5.03%</t>
+          <t>🟢 1.39%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>79.34% - 15.63% - 5.03%</t>
+          <t>96.49% - 2.12% - 1.39%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>27 (17 - 8 - 2)</t>
+          <t>19 (11 - 6 - 2)</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L5" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
@@ -1874,42 +1938,42 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>⬇ + 7d 1h</t>
+          <t>⬆ - 11d 15h</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>⬇ + 21h 36m</t>
+          <t>⬆ - 16h 42m</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>⬆ - 9h 52m</t>
+          <t>⬇ + 1h 51m</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>⬇ + 3h 23m</t>
+          <t>⬇ + 1d 10h</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>⬇ + 6d 10h</t>
+          <t>⬆ - 12d 11h</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>⬆ - 2.01%</t>
+          <t>⬆ - 13.51%</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>⬇ + 2.81%</t>
+          <t>⬆ - 3.64%</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>⬆ - 13.0</t>
+          <t>⬇ + 1.0</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -1919,7 +1983,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>⬇ + 4.0</t>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -1931,94 +1995,94 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>🔵 4d 18h</t>
+          <t>🟡 8d 12h</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>🔵 23h 21m</t>
+          <t>🟢 10h 14m</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🟢 3h 7m</t>
+          <t>🟢 3h 25m</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>🔵 10h 44m</t>
+          <t>🔵 7h 28m</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>🟡 3d 5h</t>
+          <t>🔴 7d 15h</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>🟢 7.41%</t>
+          <t>🔵 14.43%</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>🟡 6.45%</t>
+          <t>🔴 8.6%</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>86.15% - 7.41% - 6.45%</t>
+          <t>76.97% - 14.43% - 8.6%</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>96 (62 - 23 - 11)</t>
+          <t>50 (27 - 15 - 8)</t>
         </is>
       </c>
       <c r="K6" t="n">
         <v>8</v>
       </c>
       <c r="L6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M6" t="n">
         <v>21</v>
       </c>
       <c r="N6" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 12m</t>
+          <t>⬇ + 3d 17h</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>⬇ + 9h 23m</t>
+          <t>⬆ - 13h 7m</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>⬆ - 33m</t>
+          <t>⬇ + 18m</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>⬇ + 1h 36m</t>
+          <t>⬆ - 4h 9m</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>⬆ - 9h 14m</t>
+          <t>⬇ + 4d 9h</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>⬇ + 0.42%</t>
+          <t>⬇ + 7.02%</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>⬆ - 9.13%</t>
+          <t>⬇ + 2.15%</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
@@ -2028,12 +2092,12 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>⬇ + 2.0</t>
+          <t>=</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>⬆ - 1.0</t>
+          <t>⬇ - 3.0</t>
         </is>
       </c>
     </row>
@@ -2045,109 +2109,109 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>🟡 11d 14h</t>
+          <t>🔵 6d</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>🔵 1d 2h</t>
+          <t>🔵 1d 9h</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🔵 7h 22m</t>
+          <t>🟢 2h 7m</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>🔴 1d 13h</t>
+          <t>🟡 17h 31m</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>🔴 8d 15h</t>
+          <t>🟡 3d 19h</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>🔴 21.45%</t>
+          <t>🟡 17.36%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>🟡 5.41%</t>
+          <t>🔵 3.4%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>73.14% - 21.45% - 5.41%</t>
+          <t>79.25% - 17.36% - 3.4%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>75 (55 - 15 - 5)</t>
+          <t>72 (47 - 21 - 4)</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="L7" t="n">
         <v>15</v>
       </c>
       <c r="M7" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>⬇ + 3d 12h</t>
+          <t>⬆ - 5d 15h</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>⬇ + 4h 43m</t>
+          <t>⬇ + 7h 57m</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>⬇ + 2h 34m</t>
+          <t>⬆ - 5h 15m</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>⬇ + 14h 4m</t>
+          <t>⬆ - 20h 16m</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>⬇ + 2d 14h</t>
+          <t>⬆ - 4d 21h</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>⬆ - 2.3%</t>
+          <t>⬆ - 4.09%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>⬇ + 2.69%</t>
+          <t>⬆ - 2.01%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>⬇ + 4.0</t>
+          <t>⬇ + 3.0</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>⬇ + 12.0</t>
+          <t>⬆ - 1.0</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬇ - 1.0</t>
         </is>
       </c>
     </row>
@@ -2159,109 +2223,109 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>🟡 6d 17h</t>
+          <t>🟡 10d 20h</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>🟢 10h 19m</t>
+          <t>🟢 8h 4m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🟢 6h</t>
+          <t>🔵 7h 30m</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>🟡 23h 32m</t>
+          <t>🟡 18h 21m</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>🟡 5d 1h</t>
+          <t>🔴 9d 10h</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>🔵 11.11%</t>
+          <t>🔴 24.42%</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>🔵 4.32%</t>
+          <t>🔴 8.19%</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>84.57% - 11.11% - 4.32%</t>
+          <t>67.39% - 24.42% - 8.19%</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>178 (130 - 30 - 18)</t>
+          <t>82 (51 - 22 - 9)</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
         <v>1</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>⬆ - 5d 13h</t>
+          <t>⬇ + 4d 3h</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 16m</t>
+          <t>⬆ - 2h 16m</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>⬆ - 5h 47m</t>
+          <t>⬇ + 1h 26m</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>⬆ - 1d 1h</t>
+          <t>⬆ - 5h 19m</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>⬆ - 4d 1h</t>
+          <t>⬇ + 4d 9h</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>⬇ + 3.18%</t>
+          <t>⬇ + 15.54%</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
         <is>
-          <t>⬆ - 1.35%</t>
+          <t>⬇ + 4.66%</t>
         </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>⬇ + 1.0</t>
+          <t>⬇ + 2.0</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>⬇ + 1.0</t>
+          <t>⬆ - 1.0</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>⬇ + 9.0</t>
+          <t>⬇ - 7.0</t>
         </is>
       </c>
     </row>
@@ -2273,47 +2337,47 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>🔵 5d 12h</t>
+          <t>🟡 10d 1h</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🔵 1d 19h</t>
+          <t>🟢 11h 30m</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🟢 5h 14m</t>
+          <t>🟢 4h 13m</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🟡 14h 27m</t>
+          <t>🔵 9h 37m</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>🟡 2d 20h</t>
+          <t>🔴 9d</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>🔵 9.06%</t>
+          <t>🟢 3.93%</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>🟡 6.66%</t>
+          <t>🔴 16.82%</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>84.29% - 9.06% - 6.66%</t>
+          <t>79.25% - 3.93% - 16.82%</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>43 (31 - 10 - 2)</t>
+          <t>33 (22 - 9 - 2)</t>
         </is>
       </c>
       <c r="K9" t="n">
@@ -2330,37 +2394,37 @@
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>⬆ - 2d 20h</t>
+          <t>⬇ + 4d 13h</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>⬇ + 8h 41m</t>
+          <t>⬆ - 1d 8h</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>⬇ + 4h 5m</t>
+          <t>⬆ - 1h 1m</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>⬇ + 7h 44m</t>
+          <t>⬆ - 4h 50m</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>⬆ - 3d 16h</t>
+          <t>⬇ + 6d 3h</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>⬆ - 0.51%</t>
+          <t>⬆ - 5.13%</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>⬇ + 3.59%</t>
+          <t>⬇ + 10.16%</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
@@ -2375,344 +2439,344 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>⬇ + 3.0</t>
+          <t>=</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>owner_tipodecambio</t>
+          <t>owner_ticketing</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>🟡 11d 5h</t>
+          <t>🟢 16h 44m</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>🟢 4h 1m</t>
+          <t>🟢 3h 25m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🟢 32m</t>
+          <t>🟢 3h 33m</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>🟢 3h 43m</t>
+          <t>🔵 9h 46m</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>🔴 10d 21h</t>
+          <t>⚪ 0m</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>🟢 4.22%</t>
+          <t>🔵 9.99%</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>🔴 18.65%</t>
+          <t>🔵 4.29%</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>77.13% - 4.22% - 18.65%</t>
+          <t>85.72% - 9.99% - 4.29%</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>22 (6 - 13 - 3)</t>
+          <t>44 (29 - 12 - 3)</t>
         </is>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="L10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>⬇ + 3d 19h</t>
+          <t>⬇ + 16h 44m</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>⬆ - 5h 55m</t>
+          <t>⬇ + 3h 25m</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>⬆ - 3h 16m</t>
+          <t>⬇ + 3h 33m</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>⬆ - 1h 4m</t>
+          <t>⬇ + 9h 46m</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>⬇ + 4d 5h</t>
+          <t>=</t>
         </is>
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>⬇ + 1.28%</t>
+          <t>⬇ + 2.1%</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>⬆ - 3.64%</t>
+          <t>⬇ + 2.61%</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
         <is>
+          <t>⬇ + 4.0</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬆ + 1.0</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>retail</t>
+          <t>owner_tipodecambio</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>🟡 9d 4h</t>
+          <t>🔵 5d</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>🟢 14h 6m</t>
+          <t>🔵 1d 9h</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🟢 5h 44m</t>
+          <t>🟢 1h 6m</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>🟡 21h 19m</t>
+          <t>🔵 9h 40m</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>🔴 7d 11h</t>
+          <t>🟡 3d 3h</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>🟡 15.77%</t>
+          <t>🔵 12.23%</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>🟡 5.34%</t>
+          <t>🟡 6.17%</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>78.89% - 15.77% - 5.34%</t>
+          <t>81.6% - 12.23% - 6.17%</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>317 (215 - 72 - 30)</t>
+          <t>23 (10 - 12 - 1)</t>
         </is>
       </c>
       <c r="K11" t="n">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="L11" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="M11" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="N11" t="n">
         <v>1</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 3h</t>
+          <t>⬆ - 6d 5h</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>⬆ - 29m</t>
+          <t>⬇ + 1d 5h</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>⬆ - 1h 18m</t>
+          <t>⬇ + 34m</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>⬆ - 4h 49m</t>
+          <t>⬇ + 5h 57m</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>⬇ + 2d 10h</t>
+          <t>⬆ - 7d 17h</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>⬇ + 3.66%</t>
+          <t>⬇ + 8.02%</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>⬆ - 2.86%</t>
+          <t>⬆ - 12.46%</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>⬇ + 5.0</t>
+          <t>⬇ + 4.0</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>⬇ + 13.0</t>
+          <t>⬆ - 1.0</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬇ - 2.0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>financial</t>
+          <t>retail</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🟡 10d 13h</t>
+          <t>🔵 5d 7h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>🟢 17h 7m</t>
+          <t>🟢 14h 52m</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🟢 1h 32m</t>
+          <t>🟢 3h 56m</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🔵 8h 6m</t>
+          <t>🟡 21h 53m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>🔴 9d 11h</t>
+          <t>🟡 3d 14h</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>🔵 9.09%</t>
+          <t>🟡 18.08%</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>🔴 10.04%</t>
+          <t>🟡 5.79%</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>80.87% - 9.09% - 10.04%</t>
+          <t>76.13% - 18.08% - 5.79%</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>145 (85 - 44 - 16)</t>
+          <t>230 (142 - 66 - 22)</t>
         </is>
       </c>
       <c r="K12" t="n">
-        <v>8</v>
+        <v>83</v>
       </c>
       <c r="L12" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="M12" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="N12" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>⬇ + 3d 15h</t>
+          <t>⬆ - 1d 14h</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>⬇ + 8h 21m</t>
+          <t>⬇ + 4h 11m</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>⬆ - 4h 33m</t>
+          <t>⬆ - 23m</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 1h 18m</t>
+          <t>⬇ + 5h 52m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>⬇ + 3d 10h</t>
+          <t>⬆ - 2d</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>⬆ - 0.1%</t>
+          <t>⬇ + 4.84%</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>⬆ - 3.32%</t>
+          <t>⬇ + 1.56%</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>⬆ - 14.0</t>
+          <t>⬇ + 15.0</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>⬇ + 2.0</t>
+          <t>⬆ - 2.0</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
@@ -2724,109 +2788,109 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>negocios</t>
+          <t>financial</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>🔵 3d 12h</t>
+          <t>🔵 5d 20h</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>🔵 1d 7h</t>
+          <t>🟢 17h 5m</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🟢 3h 49m</t>
+          <t>🟢 2h 26m</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>🟡 14h 44m</t>
+          <t>🟡 20h 23m</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>🔵 1d 10h</t>
+          <t>🟡 4d 4h</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>🟢 6.28%</t>
+          <t>🔵 9.59%</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>🔴 11.06%</t>
+          <t>🟡 5.39%</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>82.66% - 6.28% - 11.06%</t>
+          <t>85.02% - 9.59% - 5.39%</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>60 (43 - 15 - 2)</t>
+          <t>92 (48 - 33 - 11)</t>
         </is>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L13" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="M13" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>⬆ - 1d 3h</t>
+          <t>⬆ - 4d 17h</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>⬇ + 9h 24m</t>
+          <t>⬆ - 2m</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>⬇ + 1h 3m</t>
+          <t>⬇ + 54m</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>⬇ + 5h 58m</t>
+          <t>⬇ + 11h 59m</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>⬆ - 1d 20h</t>
+          <t>⬆ - 5d 6h</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>⬆ - 0.67%</t>
+          <t>⬇ + 0.51%</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>⬆ - 11.63%</t>
+          <t>⬆ - 4.65%</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬇ + 4.0</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>⬆ - 1.0</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
@@ -2838,112 +2902,226 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>negocios</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>🟡 11d 8h</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>🟢 8h 8m</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>🟢 3h</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>🔵 11h 32m</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>🔴 10d 10h</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>🟡 15.98%</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>🔴 12.26%</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>71.76% - 15.98% - 12.26%</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>44 (24 - 13 - 7)</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>⬇ + 7d 20h</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>⬆ - 23h 31m</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>⬆ - 49m</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>⬆ - 3h 12m</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>⬇ + 8d 23h</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>⬇ + 9.7%</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>⬇ + 1.19%</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>product cx</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>🟡 6d 14h</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>🟢 11h 53m</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>🟢 4h 1m</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>🔵 12h 8m</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>🟡 5d 10h</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>🔵 9.59%</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>🔴 22.32%</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>68.09% - 9.59% - 22.32%</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>39 (18 - 12 - 9)</t>
-        </is>
-      </c>
-      <c r="K14" t="n">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>🔵 3d 17h</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>🟢 11h 12m</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>🟡 16h 17m</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>🔵 10h 44m</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>🟡 2d 3h</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>🔴 34.73%</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>🔵 4.21%</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>61.06% - 34.73% - 4.21%</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>16 (8 - 5 - 3)</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
         <v>1</v>
       </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
+      <c r="L15" t="n">
         <v>2</v>
       </c>
-      <c r="N14" t="n">
+      <c r="M15" t="n">
+        <v>4</v>
+      </c>
+      <c r="N15" t="n">
         <v>1</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>⬇ + 19h 41m</t>
-        </is>
-      </c>
-      <c r="P14" t="inlineStr">
-        <is>
-          <t>⬇ + 4h 28m</t>
-        </is>
-      </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>⬆ - 22h 20m</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>⬆ - 21h 52m</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>⬇ + 2d 11h</t>
-        </is>
-      </c>
-      <c r="T14" t="inlineStr">
-        <is>
-          <t>⬆ - 13.44%</t>
-        </is>
-      </c>
-      <c r="U14" t="inlineStr">
-        <is>
-          <t>⬇ + 18.19%</t>
-        </is>
-      </c>
-      <c r="V14" t="inlineStr">
-        <is>
-          <t>⬇ + 1.0</t>
-        </is>
-      </c>
-      <c r="W14" t="inlineStr">
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>⬆ - 2d 21h</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>⬆ - 1h 2m</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>⬇ + 12h 9m</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>⬆ - 1h 24m</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>⬆ - 3d 7h</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>⬇ + 25.14%</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>⬆ - 18.11%</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
         <is>
           <t>=</t>
         </is>
       </c>
-      <c r="X14" t="inlineStr">
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>⬇ + 3.0</t>
+        </is>
+      </c>
+      <c r="X15" t="inlineStr">
         <is>
           <t>=</t>
         </is>

</xml_diff>

<commit_message>
add lamina de restrospectiva
</commit_message>
<xml_diff>
--- a/metrics/metricas.xlsx
+++ b/metrics/metricas.xlsx
@@ -1839,7 +1839,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>⬇ + 1d 15h</t>
+          <t>⬇ + 1d 14h</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
@@ -2342,7 +2342,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>🟢 11h 30m</t>
+          <t>🟢 11h 17m</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -2679,7 +2679,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>🔵 5d 7h</t>
+          <t>🔵 5d 6h</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -2694,7 +2694,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>🟡 21h 53m</t>
+          <t>🟡 21h 41m</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -2751,7 +2751,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>⬇ + 5h 52m</t>
+          <t>⬇ + 5h 40m</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
@@ -2912,7 +2912,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>🟢 8h 8m</t>
+          <t>🟢 8h 1m</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2964,12 +2964,12 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>⬇ + 7d 20h</t>
+          <t>⬇ + 7d 19h</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>⬆ - 23h 31m</t>
+          <t>⬆ - 23h 38m</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">

</xml_diff>